<commit_message>
Fixed another minor error...
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -1,17 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="Calc"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet 1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="110">
   <si>
     <t>Broadway-7th Ave</t>
   </si>
@@ -347,33 +351,41 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="0" formatCode="General"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
-      <color indexed="8"/>
-      <name val="Helvetica"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color indexed="8"/>
-      <name val="Helvetica"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
     </font>
     <font>
-      <sz val="13"/>
-      <color indexed="8"/>
-      <name val="Helvetica"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
     </font>
     <font>
-      <b val="1"/>
       <sz val="10"/>
-      <color indexed="8"/>
-      <name val="Helvetica"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -382,1251 +394,128 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="9"/>
-        <bgColor auto="1"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="12"/>
-        <bgColor auto="1"/>
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
-    <border>
+  <borders count="2">
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right style="thin">
-        <color indexed="11"/>
-      </right>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="11"/>
-      </left>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
+  <cellStyleXfs count="20">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
   <cellXfs count="7">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="right" vertical="top"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="right" vertical="top"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="6">
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffff0000"/>
-      <rgbColor rgb="ff00ff00"/>
-      <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffffff00"/>
-      <rgbColor rgb="ffff00ff"/>
-      <rgbColor rgb="ff00ffff"/>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffdbdbdb"/>
-      <rgbColor rgb="ffa5a5a5"/>
-      <rgbColor rgb="ff3f3f3f"/>
-      <rgbColor rgb="ffffffff"/>
-    </indexedColors>
-  </colors>
 </styleSheet>
 </file>
 
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Blank">
-  <a:themeElements>
-    <a:clrScheme name="Blank">
-      <a:dk1>
-        <a:srgbClr val="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:srgbClr val="FFFFFF"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="A7A7A7"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="535353"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="499BC9"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="6EC038"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="F1D130"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="FFA93A"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="FF2D21"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="6C2085"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0000FF"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="FF00FF"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Blank">
-      <a:majorFont>
-        <a:latin typeface="Helvetica"/>
-        <a:ea typeface="Helvetica"/>
-        <a:cs typeface="Helvetica"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Helvetica"/>
-        <a:ea typeface="Helvetica"/>
-        <a:cs typeface="Helvetica"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme name="Blank">
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="35000">
-              <a:schemeClr val="phClr">
-                <a:tint val="37000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="100000"/>
-                <a:shade val="100000"/>
-                <a:satMod val="129999"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-                <a:shade val="100000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="16200000" scaled="0"/>
-        </a:gradFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr">
-              <a:shade val="95000"/>
-              <a:satMod val="104999"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="25400" dir="5400000">
-              <a:srgbClr val="000000">
-                <a:alpha val="50000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="25400" dir="5400000">
-              <a:srgbClr val="000000">
-                <a:alpha val="50000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="25400" dir="5400000">
-              <a:srgbClr val="000000">
-                <a:alpha val="50000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="40000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="40000">
-              <a:schemeClr val="phClr">
-                <a:tint val="45000"/>
-                <a:shade val="99000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="20000"/>
-                <a:satMod val="255000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
-          </a:path>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="80000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="30000"/>
-                <a:satMod val="200000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-          </a:path>
-        </a:gradFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-  <a:objectDefaults>
-    <a:spDef>
-      <a:spPr>
-        <a:solidFill>
-          <a:srgbClr val="FFFFFF"/>
-        </a:solidFill>
-        <a:ln w="25400" cap="flat">
-          <a:solidFill>
-            <a:schemeClr val="accent1"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:round/>
-        </a:ln>
-        <a:effectLst>
-          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="25400" dir="5400000">
-            <a:srgbClr val="000000">
-              <a:alpha val="50000"/>
-            </a:srgbClr>
-          </a:outerShdw>
-        </a:effectLst>
-        <a:sp3d/>
-      </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
-        <a:spAutoFit/>
-      </a:bodyPr>
-      <a:lstStyle>
-        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
-          <a:lnSpc>
-            <a:spcPct val="100000"/>
-          </a:lnSpc>
-          <a:spcBef>
-            <a:spcPts val="0"/>
-          </a:spcBef>
-          <a:spcAft>
-            <a:spcPts val="0"/>
-          </a:spcAft>
-          <a:buClrTx/>
-          <a:buSzTx/>
-          <a:buFontTx/>
-          <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:uFillTx/>
-            <a:latin typeface="+mn-lt"/>
-            <a:ea typeface="+mn-ea"/>
-            <a:cs typeface="+mn-cs"/>
-            <a:sym typeface="Helvetica"/>
-          </a:defRPr>
-        </a:defPPr>
-        <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
-          <a:lnSpc>
-            <a:spcPct val="100000"/>
-          </a:lnSpc>
-          <a:spcBef>
-            <a:spcPts val="0"/>
-          </a:spcBef>
-          <a:spcAft>
-            <a:spcPts val="0"/>
-          </a:spcAft>
-          <a:buClrTx/>
-          <a:buSzTx/>
-          <a:buFontTx/>
-          <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:uFillTx/>
-          </a:defRPr>
-        </a:lvl1pPr>
-        <a:lvl2pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
-          <a:lnSpc>
-            <a:spcPct val="100000"/>
-          </a:lnSpc>
-          <a:spcBef>
-            <a:spcPts val="0"/>
-          </a:spcBef>
-          <a:spcAft>
-            <a:spcPts val="0"/>
-          </a:spcAft>
-          <a:buClrTx/>
-          <a:buSzTx/>
-          <a:buFontTx/>
-          <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:uFillTx/>
-          </a:defRPr>
-        </a:lvl2pPr>
-        <a:lvl3pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
-          <a:lnSpc>
-            <a:spcPct val="100000"/>
-          </a:lnSpc>
-          <a:spcBef>
-            <a:spcPts val="0"/>
-          </a:spcBef>
-          <a:spcAft>
-            <a:spcPts val="0"/>
-          </a:spcAft>
-          <a:buClrTx/>
-          <a:buSzTx/>
-          <a:buFontTx/>
-          <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:uFillTx/>
-          </a:defRPr>
-        </a:lvl3pPr>
-        <a:lvl4pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
-          <a:lnSpc>
-            <a:spcPct val="100000"/>
-          </a:lnSpc>
-          <a:spcBef>
-            <a:spcPts val="0"/>
-          </a:spcBef>
-          <a:spcAft>
-            <a:spcPts val="0"/>
-          </a:spcAft>
-          <a:buClrTx/>
-          <a:buSzTx/>
-          <a:buFontTx/>
-          <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:uFillTx/>
-          </a:defRPr>
-        </a:lvl4pPr>
-        <a:lvl5pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
-          <a:lnSpc>
-            <a:spcPct val="100000"/>
-          </a:lnSpc>
-          <a:spcBef>
-            <a:spcPts val="0"/>
-          </a:spcBef>
-          <a:spcAft>
-            <a:spcPts val="0"/>
-          </a:spcAft>
-          <a:buClrTx/>
-          <a:buSzTx/>
-          <a:buFontTx/>
-          <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:uFillTx/>
-          </a:defRPr>
-        </a:lvl5pPr>
-        <a:lvl6pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
-          <a:lnSpc>
-            <a:spcPct val="100000"/>
-          </a:lnSpc>
-          <a:spcBef>
-            <a:spcPts val="0"/>
-          </a:spcBef>
-          <a:spcAft>
-            <a:spcPts val="0"/>
-          </a:spcAft>
-          <a:buClrTx/>
-          <a:buSzTx/>
-          <a:buFontTx/>
-          <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:uFillTx/>
-          </a:defRPr>
-        </a:lvl6pPr>
-        <a:lvl7pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
-          <a:lnSpc>
-            <a:spcPct val="100000"/>
-          </a:lnSpc>
-          <a:spcBef>
-            <a:spcPts val="0"/>
-          </a:spcBef>
-          <a:spcAft>
-            <a:spcPts val="0"/>
-          </a:spcAft>
-          <a:buClrTx/>
-          <a:buSzTx/>
-          <a:buFontTx/>
-          <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:uFillTx/>
-          </a:defRPr>
-        </a:lvl7pPr>
-        <a:lvl8pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
-          <a:lnSpc>
-            <a:spcPct val="100000"/>
-          </a:lnSpc>
-          <a:spcBef>
-            <a:spcPts val="0"/>
-          </a:spcBef>
-          <a:spcAft>
-            <a:spcPts val="0"/>
-          </a:spcAft>
-          <a:buClrTx/>
-          <a:buSzTx/>
-          <a:buFontTx/>
-          <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:uFillTx/>
-          </a:defRPr>
-        </a:lvl8pPr>
-        <a:lvl9pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
-          <a:lnSpc>
-            <a:spcPct val="100000"/>
-          </a:lnSpc>
-          <a:spcBef>
-            <a:spcPts val="0"/>
-          </a:spcBef>
-          <a:spcAft>
-            <a:spcPts val="0"/>
-          </a:spcAft>
-          <a:buClrTx/>
-          <a:buSzTx/>
-          <a:buFontTx/>
-          <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:uFillTx/>
-          </a:defRPr>
-        </a:lvl9pPr>
-      </a:lstStyle>
-      <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
-        <a:fontRef idx="none"/>
-      </a:style>
-    </a:spDef>
-    <a:lnDef>
-      <a:spPr>
-        <a:noFill/>
-        <a:ln w="25400" cap="flat">
-          <a:solidFill>
-            <a:schemeClr val="accent1"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:round/>
-        </a:ln>
-        <a:effectLst>
-          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="25400" dir="5400000">
-            <a:srgbClr val="000000">
-              <a:alpha val="50000"/>
-            </a:srgbClr>
-          </a:outerShdw>
-        </a:effectLst>
-        <a:sp3d/>
-      </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
-        <a:noAutofit/>
-      </a:bodyPr>
-      <a:lstStyle>
-        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
-          <a:lnSpc>
-            <a:spcPct val="100000"/>
-          </a:lnSpc>
-          <a:spcBef>
-            <a:spcPts val="0"/>
-          </a:spcBef>
-          <a:spcAft>
-            <a:spcPts val="0"/>
-          </a:spcAft>
-          <a:buClrTx/>
-          <a:buSzTx/>
-          <a:buFontTx/>
-          <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:uFillTx/>
-          </a:defRPr>
-        </a:defPPr>
-        <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
-          <a:lnSpc>
-            <a:spcPct val="100000"/>
-          </a:lnSpc>
-          <a:spcBef>
-            <a:spcPts val="0"/>
-          </a:spcBef>
-          <a:spcAft>
-            <a:spcPts val="0"/>
-          </a:spcAft>
-          <a:buClrTx/>
-          <a:buSzTx/>
-          <a:buFontTx/>
-          <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:uFillTx/>
-          </a:defRPr>
-        </a:lvl1pPr>
-        <a:lvl2pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
-          <a:lnSpc>
-            <a:spcPct val="100000"/>
-          </a:lnSpc>
-          <a:spcBef>
-            <a:spcPts val="0"/>
-          </a:spcBef>
-          <a:spcAft>
-            <a:spcPts val="0"/>
-          </a:spcAft>
-          <a:buClrTx/>
-          <a:buSzTx/>
-          <a:buFontTx/>
-          <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:uFillTx/>
-          </a:defRPr>
-        </a:lvl2pPr>
-        <a:lvl3pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
-          <a:lnSpc>
-            <a:spcPct val="100000"/>
-          </a:lnSpc>
-          <a:spcBef>
-            <a:spcPts val="0"/>
-          </a:spcBef>
-          <a:spcAft>
-            <a:spcPts val="0"/>
-          </a:spcAft>
-          <a:buClrTx/>
-          <a:buSzTx/>
-          <a:buFontTx/>
-          <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:uFillTx/>
-          </a:defRPr>
-        </a:lvl3pPr>
-        <a:lvl4pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
-          <a:lnSpc>
-            <a:spcPct val="100000"/>
-          </a:lnSpc>
-          <a:spcBef>
-            <a:spcPts val="0"/>
-          </a:spcBef>
-          <a:spcAft>
-            <a:spcPts val="0"/>
-          </a:spcAft>
-          <a:buClrTx/>
-          <a:buSzTx/>
-          <a:buFontTx/>
-          <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:uFillTx/>
-          </a:defRPr>
-        </a:lvl4pPr>
-        <a:lvl5pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
-          <a:lnSpc>
-            <a:spcPct val="100000"/>
-          </a:lnSpc>
-          <a:spcBef>
-            <a:spcPts val="0"/>
-          </a:spcBef>
-          <a:spcAft>
-            <a:spcPts val="0"/>
-          </a:spcAft>
-          <a:buClrTx/>
-          <a:buSzTx/>
-          <a:buFontTx/>
-          <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:uFillTx/>
-          </a:defRPr>
-        </a:lvl5pPr>
-        <a:lvl6pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
-          <a:lnSpc>
-            <a:spcPct val="100000"/>
-          </a:lnSpc>
-          <a:spcBef>
-            <a:spcPts val="0"/>
-          </a:spcBef>
-          <a:spcAft>
-            <a:spcPts val="0"/>
-          </a:spcAft>
-          <a:buClrTx/>
-          <a:buSzTx/>
-          <a:buFontTx/>
-          <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:uFillTx/>
-          </a:defRPr>
-        </a:lvl6pPr>
-        <a:lvl7pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
-          <a:lnSpc>
-            <a:spcPct val="100000"/>
-          </a:lnSpc>
-          <a:spcBef>
-            <a:spcPts val="0"/>
-          </a:spcBef>
-          <a:spcAft>
-            <a:spcPts val="0"/>
-          </a:spcAft>
-          <a:buClrTx/>
-          <a:buSzTx/>
-          <a:buFontTx/>
-          <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:uFillTx/>
-          </a:defRPr>
-        </a:lvl7pPr>
-        <a:lvl8pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
-          <a:lnSpc>
-            <a:spcPct val="100000"/>
-          </a:lnSpc>
-          <a:spcBef>
-            <a:spcPts val="0"/>
-          </a:spcBef>
-          <a:spcAft>
-            <a:spcPts val="0"/>
-          </a:spcAft>
-          <a:buClrTx/>
-          <a:buSzTx/>
-          <a:buFontTx/>
-          <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:uFillTx/>
-          </a:defRPr>
-        </a:lvl8pPr>
-        <a:lvl9pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
-          <a:lnSpc>
-            <a:spcPct val="100000"/>
-          </a:lnSpc>
-          <a:spcBef>
-            <a:spcPts val="0"/>
-          </a:spcBef>
-          <a:spcAft>
-            <a:spcPts val="0"/>
-          </a:spcAft>
-          <a:buClrTx/>
-          <a:buSzTx/>
-          <a:buFontTx/>
-          <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:uFillTx/>
-          </a:defRPr>
-        </a:lvl9pPr>
-      </a:lstStyle>
-      <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
-        <a:fontRef idx="none"/>
-      </a:style>
-    </a:lnDef>
-    <a:txDef>
-      <a:spPr>
-        <a:noFill/>
-        <a:ln w="12700" cap="flat">
-          <a:noFill/>
-          <a:miter lim="400000"/>
-        </a:ln>
-        <a:effectLst/>
-        <a:sp3d/>
-      </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
-        <a:spAutoFit/>
-      </a:bodyPr>
-      <a:lstStyle>
-        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
-          <a:lnSpc>
-            <a:spcPct val="100000"/>
-          </a:lnSpc>
-          <a:spcBef>
-            <a:spcPts val="0"/>
-          </a:spcBef>
-          <a:spcAft>
-            <a:spcPts val="0"/>
-          </a:spcAft>
-          <a:buClrTx/>
-          <a:buSzTx/>
-          <a:buFontTx/>
-          <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:uFillTx/>
-            <a:latin typeface="+mn-lt"/>
-            <a:ea typeface="+mn-ea"/>
-            <a:cs typeface="+mn-cs"/>
-            <a:sym typeface="Helvetica"/>
-          </a:defRPr>
-        </a:defPPr>
-        <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
-          <a:lnSpc>
-            <a:spcPct val="100000"/>
-          </a:lnSpc>
-          <a:spcBef>
-            <a:spcPts val="0"/>
-          </a:spcBef>
-          <a:spcAft>
-            <a:spcPts val="0"/>
-          </a:spcAft>
-          <a:buClrTx/>
-          <a:buSzTx/>
-          <a:buFontTx/>
-          <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:uFillTx/>
-          </a:defRPr>
-        </a:lvl1pPr>
-        <a:lvl2pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
-          <a:lnSpc>
-            <a:spcPct val="100000"/>
-          </a:lnSpc>
-          <a:spcBef>
-            <a:spcPts val="0"/>
-          </a:spcBef>
-          <a:spcAft>
-            <a:spcPts val="0"/>
-          </a:spcAft>
-          <a:buClrTx/>
-          <a:buSzTx/>
-          <a:buFontTx/>
-          <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:uFillTx/>
-          </a:defRPr>
-        </a:lvl2pPr>
-        <a:lvl3pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
-          <a:lnSpc>
-            <a:spcPct val="100000"/>
-          </a:lnSpc>
-          <a:spcBef>
-            <a:spcPts val="0"/>
-          </a:spcBef>
-          <a:spcAft>
-            <a:spcPts val="0"/>
-          </a:spcAft>
-          <a:buClrTx/>
-          <a:buSzTx/>
-          <a:buFontTx/>
-          <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:uFillTx/>
-          </a:defRPr>
-        </a:lvl3pPr>
-        <a:lvl4pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
-          <a:lnSpc>
-            <a:spcPct val="100000"/>
-          </a:lnSpc>
-          <a:spcBef>
-            <a:spcPts val="0"/>
-          </a:spcBef>
-          <a:spcAft>
-            <a:spcPts val="0"/>
-          </a:spcAft>
-          <a:buClrTx/>
-          <a:buSzTx/>
-          <a:buFontTx/>
-          <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:uFillTx/>
-          </a:defRPr>
-        </a:lvl4pPr>
-        <a:lvl5pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
-          <a:lnSpc>
-            <a:spcPct val="100000"/>
-          </a:lnSpc>
-          <a:spcBef>
-            <a:spcPts val="0"/>
-          </a:spcBef>
-          <a:spcAft>
-            <a:spcPts val="0"/>
-          </a:spcAft>
-          <a:buClrTx/>
-          <a:buSzTx/>
-          <a:buFontTx/>
-          <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:uFillTx/>
-          </a:defRPr>
-        </a:lvl5pPr>
-        <a:lvl6pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
-          <a:lnSpc>
-            <a:spcPct val="100000"/>
-          </a:lnSpc>
-          <a:spcBef>
-            <a:spcPts val="0"/>
-          </a:spcBef>
-          <a:spcAft>
-            <a:spcPts val="0"/>
-          </a:spcAft>
-          <a:buClrTx/>
-          <a:buSzTx/>
-          <a:buFontTx/>
-          <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:uFillTx/>
-          </a:defRPr>
-        </a:lvl6pPr>
-        <a:lvl7pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
-          <a:lnSpc>
-            <a:spcPct val="100000"/>
-          </a:lnSpc>
-          <a:spcBef>
-            <a:spcPts val="0"/>
-          </a:spcBef>
-          <a:spcAft>
-            <a:spcPts val="0"/>
-          </a:spcAft>
-          <a:buClrTx/>
-          <a:buSzTx/>
-          <a:buFontTx/>
-          <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:uFillTx/>
-          </a:defRPr>
-        </a:lvl7pPr>
-        <a:lvl8pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
-          <a:lnSpc>
-            <a:spcPct val="100000"/>
-          </a:lnSpc>
-          <a:spcBef>
-            <a:spcPts val="0"/>
-          </a:spcBef>
-          <a:spcAft>
-            <a:spcPts val="0"/>
-          </a:spcAft>
-          <a:buClrTx/>
-          <a:buSzTx/>
-          <a:buFontTx/>
-          <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:uFillTx/>
-          </a:defRPr>
-        </a:lvl8pPr>
-        <a:lvl9pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
-          <a:lnSpc>
-            <a:spcPct val="100000"/>
-          </a:lnSpc>
-          <a:spcBef>
-            <a:spcPts val="0"/>
-          </a:spcBef>
-          <a:spcAft>
-            <a:spcPts val="0"/>
-          </a:spcAft>
-          <a:buClrTx/>
-          <a:buSzTx/>
-          <a:buFontTx/>
-          <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:uFillTx/>
-          </a:defRPr>
-        </a:lvl9pPr>
-      </a:lstStyle>
-      <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
-        <a:fontRef idx="none"/>
-      </a:style>
-    </a:txDef>
-  </a:objectDefaults>
-</a:theme>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <pageSetUpPr fitToPage="1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="true"/>
   </sheetPr>
   <dimension ref="A1:O115"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="162" zoomScaleNormal="162" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="P14" activeCellId="0" sqref="P14"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.33333" defaultRowHeight="18" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="18"/>
   <cols>
-    <col min="1" max="1" width="16.6719" style="1" customWidth="1"/>
-    <col min="2" max="2" width="8.35156" style="1" customWidth="1"/>
-    <col min="3" max="3" width="27.8516" style="1" customWidth="1"/>
-    <col min="4" max="4" width="2.85156" style="1" customWidth="1"/>
-    <col min="5" max="5" width="3" style="1" customWidth="1"/>
-    <col min="6" max="6" width="3" style="1" customWidth="1"/>
-    <col min="7" max="7" width="3" style="1" customWidth="1"/>
-    <col min="8" max="8" width="3" style="1" customWidth="1"/>
-    <col min="9" max="9" width="3" style="1" customWidth="1"/>
-    <col min="10" max="10" width="3" style="1" customWidth="1"/>
-    <col min="11" max="11" width="2.67188" style="1" customWidth="1"/>
-    <col min="12" max="12" width="2.85156" style="1" customWidth="1"/>
-    <col min="13" max="13" width="2.67188" style="1" customWidth="1"/>
-    <col min="14" max="14" width="2.67188" style="1" customWidth="1"/>
-    <col min="15" max="15" width="3" style="1" customWidth="1"/>
-    <col min="16" max="256" width="8.35156" style="1" customWidth="1"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="16.6734693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="8.35204081632653"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="27.8520408163265"/>
+    <col collapsed="false" hidden="false" max="15" min="4" style="1" width="3.51020408163265"/>
+    <col collapsed="false" hidden="false" max="256" min="16" style="1" width="8.35204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="257" style="0" width="8.33163265306122"/>
   </cols>
   <sheetData>
-    <row r="1" ht="20.35" customHeight="1">
-      <c r="A1" t="s" s="2">
+    <row r="1" customFormat="false" ht="20.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3">
+      <c r="B1" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="4">
+      <c r="C1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="5">
+      <c r="D1" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="E1" t="s" s="6">
+      <c r="E1" s="6" t="s">
         <v>2</v>
       </c>
       <c r="F1" s="5"/>
@@ -1640,17 +529,17 @@
       <c r="N1" s="5"/>
       <c r="O1" s="5"/>
     </row>
-    <row r="2" ht="20.35" customHeight="1">
-      <c r="A2" t="s" s="2">
+    <row r="2" customFormat="false" ht="20.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="C2" t="s" s="4">
+      <c r="C2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="5">
+      <c r="D2" s="5" t="n">
         <v>1</v>
       </c>
       <c r="E2" s="5"/>
@@ -1665,23 +554,23 @@
       <c r="N2" s="5"/>
       <c r="O2" s="5"/>
     </row>
-    <row r="3" ht="20.35" customHeight="1">
-      <c r="A3" t="s" s="2">
+    <row r="3" customFormat="false" ht="20.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="C3" t="s" s="4">
+      <c r="C3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F3" s="5" t="n">
         <v>3</v>
       </c>
       <c r="G3" s="5"/>
@@ -1694,17 +583,17 @@
       <c r="N3" s="5"/>
       <c r="O3" s="5"/>
     </row>
-    <row r="4" ht="20.35" customHeight="1">
-      <c r="A4" t="s" s="2">
+    <row r="4" customFormat="false" ht="20.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="C4" t="s" s="4">
+      <c r="C4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="5" t="n">
         <v>1</v>
       </c>
       <c r="E4" s="5"/>
@@ -1719,17 +608,17 @@
       <c r="N4" s="5"/>
       <c r="O4" s="5"/>
     </row>
-    <row r="5" ht="20.35" customHeight="1">
-      <c r="A5" t="s" s="2">
+    <row r="5" customFormat="false" ht="20.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="C5" t="s" s="4">
+      <c r="C5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="5" t="n">
         <v>1</v>
       </c>
       <c r="E5" s="5"/>
@@ -1744,17 +633,17 @@
       <c r="N5" s="5"/>
       <c r="O5" s="5"/>
     </row>
-    <row r="6" ht="20.35" customHeight="1">
-      <c r="A6" t="s" s="2">
+    <row r="6" customFormat="false" ht="20.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="C6" t="s" s="4">
+      <c r="C6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="5" t="n">
         <v>1</v>
       </c>
       <c r="E6" s="5"/>
@@ -1769,17 +658,17 @@
       <c r="N6" s="5"/>
       <c r="O6" s="5"/>
     </row>
-    <row r="7" ht="20.35" customHeight="1">
-      <c r="A7" t="s" s="2">
+    <row r="7" customFormat="false" ht="20.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="C7" t="s" s="4">
+      <c r="C7" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="5" t="n">
         <v>1</v>
       </c>
       <c r="E7" s="5"/>
@@ -1794,32 +683,32 @@
       <c r="N7" s="5"/>
       <c r="O7" s="5"/>
     </row>
-    <row r="8" ht="20.35" customHeight="1">
-      <c r="A8" t="s" s="2">
+    <row r="8" customFormat="false" ht="20.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="C8" t="s" s="4">
+      <c r="C8" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E8" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F8" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="G8" t="s" s="6">
+      <c r="G8" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="H8" t="s" s="6">
+      <c r="H8" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="I8" t="s" s="6">
+      <c r="I8" s="6" t="s">
         <v>12</v>
       </c>
       <c r="J8" s="5"/>
@@ -1829,17 +718,17 @@
       <c r="N8" s="5"/>
       <c r="O8" s="5"/>
     </row>
-    <row r="9" ht="20.35" customHeight="1">
-      <c r="A9" t="s" s="2">
+    <row r="9" customFormat="false" ht="20.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="3" t="n">
         <v>9</v>
       </c>
-      <c r="C9" t="s" s="4">
+      <c r="C9" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="5" t="n">
         <v>1</v>
       </c>
       <c r="E9" s="5"/>
@@ -1854,17 +743,17 @@
       <c r="N9" s="5"/>
       <c r="O9" s="5"/>
     </row>
-    <row r="10" ht="20.35" customHeight="1">
-      <c r="A10" t="s" s="2">
+    <row r="10" customFormat="false" ht="20.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10" s="3" t="n">
         <v>10</v>
       </c>
-      <c r="C10" t="s" s="4">
+      <c r="C10" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10" s="5" t="n">
         <v>1</v>
       </c>
       <c r="E10" s="5"/>
@@ -1879,17 +768,17 @@
       <c r="N10" s="5"/>
       <c r="O10" s="5"/>
     </row>
-    <row r="11" ht="20.35" customHeight="1">
-      <c r="A11" t="s" s="2">
+    <row r="11" customFormat="false" ht="20.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B11" s="3" t="n">
         <v>11</v>
       </c>
-      <c r="C11" t="s" s="4">
+      <c r="C11" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D11" s="5" t="n">
         <v>1</v>
       </c>
       <c r="E11" s="5"/>
@@ -1904,23 +793,23 @@
       <c r="N11" s="5"/>
       <c r="O11" s="5"/>
     </row>
-    <row r="12" ht="20.35" customHeight="1">
-      <c r="A12" t="s" s="2">
+    <row r="12" customFormat="false" ht="20.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B12" s="3" t="n">
         <v>12</v>
       </c>
-      <c r="C12" t="s" s="4">
+      <c r="C12" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="5">
+      <c r="D12" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="E12" s="5">
+      <c r="E12" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="F12" s="5">
+      <c r="F12" s="5" t="n">
         <v>3</v>
       </c>
       <c r="G12" s="5"/>
@@ -1933,64 +822,64 @@
       <c r="N12" s="5"/>
       <c r="O12" s="5"/>
     </row>
-    <row r="13" ht="20.35" customHeight="1">
-      <c r="A13" t="s" s="2">
+    <row r="13" customFormat="false" ht="20.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B13" s="3">
+      <c r="B13" s="3" t="n">
         <v>13</v>
       </c>
-      <c r="C13" t="s" s="4">
+      <c r="C13" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D13" s="5">
+      <c r="D13" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="E13" s="5">
+      <c r="E13" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="F13" s="5">
+      <c r="F13" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="G13" s="5">
+      <c r="G13" s="5" t="n">
         <v>7</v>
       </c>
-      <c r="H13" t="s" s="6">
+      <c r="H13" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="I13" t="s" s="6">
+      <c r="I13" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="J13" t="s" s="6">
+      <c r="J13" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="K13" t="s" s="6">
+      <c r="K13" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="L13" t="s" s="6">
+      <c r="L13" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="M13" t="s" s="6">
+      <c r="M13" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="N13" t="s" s="6">
+      <c r="N13" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="O13" t="s" s="6">
+      <c r="O13" s="6" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="14" ht="20.35" customHeight="1">
-      <c r="A14" t="s" s="2">
+    <row r="14" customFormat="false" ht="20.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B14" s="3">
+      <c r="B14" s="3" t="n">
         <v>14</v>
       </c>
-      <c r="C14" t="s" s="4">
+      <c r="C14" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D14" s="5">
+      <c r="D14" s="5" t="n">
         <v>1</v>
       </c>
       <c r="E14" s="5"/>
@@ -2005,29 +894,29 @@
       <c r="N14" s="5"/>
       <c r="O14" s="5"/>
     </row>
-    <row r="15" ht="20.35" customHeight="1">
-      <c r="A15" t="s" s="2">
+    <row r="15" customFormat="false" ht="20.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B15" s="3">
+      <c r="B15" s="3" t="n">
         <v>15</v>
       </c>
-      <c r="C15" t="s" s="4">
+      <c r="C15" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D15" s="5">
+      <c r="D15" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="E15" t="s" s="6">
+      <c r="E15" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="F15" t="s" s="6">
+      <c r="F15" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="G15" t="s" s="6">
+      <c r="G15" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="H15" t="s" s="6">
+      <c r="H15" s="6" t="s">
         <v>28</v>
       </c>
       <c r="I15" s="5"/>
@@ -2038,17 +927,17 @@
       <c r="N15" s="5"/>
       <c r="O15" s="5"/>
     </row>
-    <row r="16" ht="20.35" customHeight="1">
-      <c r="A16" t="s" s="2">
+    <row r="16" customFormat="false" ht="20.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B16" s="3">
+      <c r="B16" s="3" t="n">
         <v>16</v>
       </c>
-      <c r="C16" t="s" s="4">
+      <c r="C16" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D16" s="5">
+      <c r="D16" s="5" t="n">
         <v>1</v>
       </c>
       <c r="E16" s="5"/>
@@ -2063,23 +952,23 @@
       <c r="N16" s="5"/>
       <c r="O16" s="5"/>
     </row>
-    <row r="17" ht="20.35" customHeight="1">
-      <c r="A17" t="s" s="2">
+    <row r="17" customFormat="false" ht="20.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B17" s="3">
+      <c r="B17" s="3" t="n">
         <v>17</v>
       </c>
-      <c r="C17" t="s" s="4">
+      <c r="C17" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="D17" s="5">
+      <c r="D17" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="E17" s="5">
+      <c r="E17" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="F17" s="5">
+      <c r="F17" s="5" t="n">
         <v>3</v>
       </c>
       <c r="G17" s="5"/>
@@ -2092,17 +981,17 @@
       <c r="N17" s="5"/>
       <c r="O17" s="5"/>
     </row>
-    <row r="18" ht="20.35" customHeight="1">
-      <c r="A18" t="s" s="2">
+    <row r="18" customFormat="false" ht="20.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A18" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B18" s="3">
+      <c r="B18" s="3" t="n">
         <v>18</v>
       </c>
-      <c r="C18" t="s" s="4">
+      <c r="C18" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="D18" s="5">
+      <c r="D18" s="5" t="n">
         <v>1</v>
       </c>
       <c r="E18" s="5"/>
@@ -2117,17 +1006,17 @@
       <c r="N18" s="5"/>
       <c r="O18" s="5"/>
     </row>
-    <row r="19" ht="20.35" customHeight="1">
-      <c r="A19" t="s" s="2">
+    <row r="19" customFormat="false" ht="20.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B19" s="3">
+      <c r="B19" s="3" t="n">
         <v>19</v>
       </c>
-      <c r="C19" t="s" s="4">
+      <c r="C19" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D19" s="5">
+      <c r="D19" s="5" t="n">
         <v>1</v>
       </c>
       <c r="E19" s="5"/>
@@ -2142,23 +1031,23 @@
       <c r="N19" s="5"/>
       <c r="O19" s="5"/>
     </row>
-    <row r="20" ht="20.35" customHeight="1">
-      <c r="A20" t="s" s="2">
+    <row r="20" customFormat="false" ht="20.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B20" s="3">
+      <c r="B20" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="C20" t="s" s="4">
+      <c r="C20" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="D20" s="5">
+      <c r="D20" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="E20" s="5">
+      <c r="E20" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="F20" s="5">
+      <c r="F20" s="5" t="n">
         <v>3</v>
       </c>
       <c r="G20" s="5"/>
@@ -2171,17 +1060,17 @@
       <c r="N20" s="5"/>
       <c r="O20" s="5"/>
     </row>
-    <row r="21" ht="20.35" customHeight="1">
-      <c r="A21" t="s" s="2">
+    <row r="21" customFormat="false" ht="20.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A21" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B21" s="3">
+      <c r="B21" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="C21" t="s" s="4">
+      <c r="C21" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="D21" s="5">
+      <c r="D21" s="5" t="n">
         <v>1</v>
       </c>
       <c r="E21" s="5"/>
@@ -2196,17 +1085,17 @@
       <c r="N21" s="5"/>
       <c r="O21" s="5"/>
     </row>
-    <row r="22" ht="20.35" customHeight="1">
-      <c r="A22" t="s" s="2">
+    <row r="22" customFormat="false" ht="20.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A22" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B22" s="3">
+      <c r="B22" s="3" t="n">
         <v>22</v>
       </c>
-      <c r="C22" t="s" s="4">
+      <c r="C22" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D22" s="5">
+      <c r="D22" s="5" t="n">
         <v>1</v>
       </c>
       <c r="E22" s="5"/>
@@ -2221,17 +1110,17 @@
       <c r="N22" s="5"/>
       <c r="O22" s="5"/>
     </row>
-    <row r="23" ht="20.35" customHeight="1">
-      <c r="A23" t="s" s="2">
+    <row r="23" customFormat="false" ht="20.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A23" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B23" s="3">
+      <c r="B23" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="C23" t="s" s="4">
+      <c r="C23" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="D23" s="5">
+      <c r="D23" s="5" t="n">
         <v>1</v>
       </c>
       <c r="E23" s="5"/>
@@ -2246,17 +1135,17 @@
       <c r="N23" s="5"/>
       <c r="O23" s="5"/>
     </row>
-    <row r="24" ht="20.35" customHeight="1">
-      <c r="A24" t="s" s="2">
+    <row r="24" customFormat="false" ht="20.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A24" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B24" s="3">
+      <c r="B24" s="3" t="n">
         <v>24</v>
       </c>
-      <c r="C24" t="s" s="4">
+      <c r="C24" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="D24" s="5">
+      <c r="D24" s="5" t="n">
         <v>1</v>
       </c>
       <c r="E24" s="5"/>
@@ -2271,17 +1160,17 @@
       <c r="N24" s="5"/>
       <c r="O24" s="5"/>
     </row>
-    <row r="25" ht="20.35" customHeight="1">
-      <c r="A25" t="s" s="2">
+    <row r="25" customFormat="false" ht="20.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A25" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B25" s="3">
+      <c r="B25" s="3" t="n">
         <v>25</v>
       </c>
-      <c r="C25" t="s" s="4">
+      <c r="C25" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="D25" s="5">
+      <c r="D25" s="5" t="n">
         <v>1</v>
       </c>
       <c r="E25" s="5"/>
@@ -2296,17 +1185,17 @@
       <c r="N25" s="5"/>
       <c r="O25" s="5"/>
     </row>
-    <row r="26" ht="20.35" customHeight="1">
-      <c r="A26" t="s" s="2">
+    <row r="26" customFormat="false" ht="20.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A26" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B26" s="3">
+      <c r="B26" s="3" t="n">
         <v>26</v>
       </c>
-      <c r="C26" t="s" s="4">
+      <c r="C26" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="D26" s="5">
+      <c r="D26" s="5" t="n">
         <v>1</v>
       </c>
       <c r="E26" s="5"/>
@@ -2321,17 +1210,17 @@
       <c r="N26" s="5"/>
       <c r="O26" s="5"/>
     </row>
-    <row r="27" ht="20.35" customHeight="1">
-      <c r="A27" t="s" s="2">
+    <row r="27" customFormat="false" ht="20.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A27" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="3">
+      <c r="B27" s="3" t="n">
         <v>27</v>
       </c>
-      <c r="C27" t="s" s="4">
+      <c r="C27" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="D27" s="5">
+      <c r="D27" s="5" t="n">
         <v>1</v>
       </c>
       <c r="E27" s="5"/>
@@ -2346,23 +1235,23 @@
       <c r="N27" s="5"/>
       <c r="O27" s="5"/>
     </row>
-    <row r="28" ht="20.35" customHeight="1">
-      <c r="A28" t="s" s="2">
+    <row r="28" customFormat="false" ht="20.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A28" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="3">
+      <c r="B28" s="3" t="n">
         <v>28</v>
       </c>
-      <c r="C28" t="s" s="4">
+      <c r="C28" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="D28" s="5">
+      <c r="D28" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="E28" t="s" s="6">
+      <c r="E28" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="F28" t="s" s="6">
+      <c r="F28" s="6" t="s">
         <v>19</v>
       </c>
       <c r="G28" s="5"/>
@@ -2375,17 +1264,17 @@
       <c r="N28" s="5"/>
       <c r="O28" s="5"/>
     </row>
-    <row r="29" ht="20.35" customHeight="1">
-      <c r="A29" t="s" s="2">
+    <row r="29" customFormat="false" ht="20.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A29" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B29" s="3">
+      <c r="B29" s="3" t="n">
         <v>29</v>
       </c>
-      <c r="C29" t="s" s="4">
+      <c r="C29" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="D29" s="5">
+      <c r="D29" s="5" t="n">
         <v>1</v>
       </c>
       <c r="E29" s="5"/>
@@ -2400,17 +1289,17 @@
       <c r="N29" s="5"/>
       <c r="O29" s="5"/>
     </row>
-    <row r="30" ht="20.35" customHeight="1">
-      <c r="A30" t="s" s="2">
+    <row r="30" customFormat="false" ht="20.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A30" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B30" s="3">
+      <c r="B30" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="C30" t="s" s="4">
+      <c r="C30" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="D30" s="5">
+      <c r="D30" s="5" t="n">
         <v>1</v>
       </c>
       <c r="E30" s="5"/>
@@ -2425,17 +1314,17 @@
       <c r="N30" s="5"/>
       <c r="O30" s="5"/>
     </row>
-    <row r="31" ht="20.35" customHeight="1">
-      <c r="A31" t="s" s="2">
+    <row r="31" customFormat="false" ht="20.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A31" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B31" s="3">
+      <c r="B31" s="3" t="n">
         <v>31</v>
       </c>
-      <c r="C31" t="s" s="4">
+      <c r="C31" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="D31" s="5">
+      <c r="D31" s="5" t="n">
         <v>1</v>
       </c>
       <c r="E31" s="5"/>
@@ -2450,17 +1339,17 @@
       <c r="N31" s="5"/>
       <c r="O31" s="5"/>
     </row>
-    <row r="32" ht="20.35" customHeight="1">
-      <c r="A32" t="s" s="2">
+    <row r="32" customFormat="false" ht="20.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A32" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B32" s="3">
+      <c r="B32" s="3" t="n">
         <v>32</v>
       </c>
-      <c r="C32" t="s" s="4">
+      <c r="C32" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="D32" s="5">
+      <c r="D32" s="5" t="n">
         <v>1</v>
       </c>
       <c r="E32" s="5"/>
@@ -2475,17 +1364,17 @@
       <c r="N32" s="5"/>
       <c r="O32" s="5"/>
     </row>
-    <row r="33" ht="20.35" customHeight="1">
-      <c r="A33" t="s" s="2">
+    <row r="33" customFormat="false" ht="20.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A33" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B33" s="3">
+      <c r="B33" s="3" t="n">
         <v>33</v>
       </c>
-      <c r="C33" t="s" s="4">
+      <c r="C33" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="D33" s="5">
+      <c r="D33" s="5" t="n">
         <v>1</v>
       </c>
       <c r="E33" s="5"/>
@@ -2500,20 +1389,20 @@
       <c r="N33" s="5"/>
       <c r="O33" s="5"/>
     </row>
-    <row r="34" ht="20.35" customHeight="1">
-      <c r="A34" t="s" s="2">
+    <row r="34" customFormat="false" ht="20.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A34" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B34" s="3">
+      <c r="B34" s="3" t="n">
         <v>34</v>
       </c>
-      <c r="C34" t="s" s="4">
+      <c r="C34" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="D34" s="5">
+      <c r="D34" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="E34" s="5">
+      <c r="E34" s="5" t="n">
         <v>3</v>
       </c>
       <c r="F34" s="5"/>
@@ -2527,38 +1416,38 @@
       <c r="N34" s="5"/>
       <c r="O34" s="5"/>
     </row>
-    <row r="35" ht="20.35" customHeight="1">
-      <c r="A35" t="s" s="2">
+    <row r="35" customFormat="false" ht="20.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A35" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B35" s="3">
+      <c r="B35" s="3" t="n">
         <v>35</v>
       </c>
-      <c r="C35" t="s" s="4">
+      <c r="C35" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="D35" s="5">
+      <c r="D35" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="E35" s="5">
+      <c r="E35" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="F35" s="5">
+      <c r="F35" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="G35" s="5">
+      <c r="G35" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="H35" t="s" s="6">
+      <c r="H35" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="I35" t="s" s="6">
+      <c r="I35" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="J35" t="s" s="6">
+      <c r="J35" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="K35" t="s" s="6">
+      <c r="K35" s="6" t="s">
         <v>51</v>
       </c>
       <c r="L35" s="5"/>
@@ -2566,29 +1455,29 @@
       <c r="N35" s="5"/>
       <c r="O35" s="5"/>
     </row>
-    <row r="36" ht="20.35" customHeight="1">
-      <c r="A36" t="s" s="2">
+    <row r="36" customFormat="false" ht="20.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A36" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B36" s="3">
+      <c r="B36" s="3" t="n">
         <v>36</v>
       </c>
-      <c r="C36" t="s" s="4">
+      <c r="C36" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="D36" s="5">
+      <c r="D36" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="E36" s="5">
+      <c r="E36" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="F36" t="s" s="6">
+      <c r="F36" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="G36" t="s" s="6">
+      <c r="G36" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="H36" t="s" s="6">
+      <c r="H36" s="6" t="s">
         <v>20</v>
       </c>
       <c r="I36" s="5"/>
@@ -2599,20 +1488,20 @@
       <c r="N36" s="5"/>
       <c r="O36" s="5"/>
     </row>
-    <row r="37" ht="20.35" customHeight="1">
-      <c r="A37" t="s" s="2">
+    <row r="37" customFormat="false" ht="20.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A37" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B37" s="3">
+      <c r="B37" s="3" t="n">
         <v>37</v>
       </c>
-      <c r="C37" t="s" s="4">
+      <c r="C37" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="D37" s="5">
+      <c r="D37" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="E37" s="5">
+      <c r="E37" s="5" t="n">
         <v>3</v>
       </c>
       <c r="F37" s="5"/>
@@ -2626,20 +1515,20 @@
       <c r="N37" s="5"/>
       <c r="O37" s="5"/>
     </row>
-    <row r="38" ht="20.35" customHeight="1">
-      <c r="A38" t="s" s="2">
+    <row r="38" customFormat="false" ht="20.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A38" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B38" s="3">
+      <c r="B38" s="3" t="n">
         <v>38</v>
       </c>
-      <c r="C38" t="s" s="4">
+      <c r="C38" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="D38" s="5">
+      <c r="D38" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="E38" s="5">
+      <c r="E38" s="5" t="n">
         <v>3</v>
       </c>
       <c r="F38" s="5"/>
@@ -2653,20 +1542,20 @@
       <c r="N38" s="5"/>
       <c r="O38" s="5"/>
     </row>
-    <row r="39" ht="20.35" customHeight="1">
-      <c r="A39" t="s" s="2">
+    <row r="39" customFormat="false" ht="20.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A39" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B39" s="3">
+      <c r="B39" s="3" t="n">
         <v>39</v>
       </c>
-      <c r="C39" t="s" s="4">
+      <c r="C39" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="D39" s="5">
+      <c r="D39" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="E39" s="5">
+      <c r="E39" s="5" t="n">
         <v>3</v>
       </c>
       <c r="F39" s="5"/>
@@ -2680,20 +1569,20 @@
       <c r="N39" s="5"/>
       <c r="O39" s="5"/>
     </row>
-    <row r="40" ht="20.35" customHeight="1">
-      <c r="A40" t="s" s="2">
+    <row r="40" customFormat="false" ht="20.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A40" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B40" s="3">
+      <c r="B40" s="3" t="n">
         <v>40</v>
       </c>
-      <c r="C40" t="s" s="4">
+      <c r="C40" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="D40" s="5">
+      <c r="D40" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="E40" s="5">
+      <c r="E40" s="5" t="n">
         <v>3</v>
       </c>
       <c r="F40" s="5"/>
@@ -2707,17 +1596,17 @@
       <c r="N40" s="5"/>
       <c r="O40" s="5"/>
     </row>
-    <row r="41" ht="20.35" customHeight="1">
-      <c r="A41" t="s" s="2">
+    <row r="41" customFormat="false" ht="20.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A41" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B41" s="3">
+      <c r="B41" s="3" t="n">
         <v>41</v>
       </c>
-      <c r="C41" t="s" s="4">
+      <c r="C41" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="D41" s="5">
+      <c r="D41" s="5" t="n">
         <v>3</v>
       </c>
       <c r="E41" s="5"/>
@@ -2732,17 +1621,17 @@
       <c r="N41" s="5"/>
       <c r="O41" s="5"/>
     </row>
-    <row r="42" ht="20.35" customHeight="1">
-      <c r="A42" t="s" s="2">
+    <row r="42" customFormat="false" ht="20.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A42" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B42" s="3">
+      <c r="B42" s="3" t="n">
         <v>42</v>
       </c>
-      <c r="C42" t="s" s="4">
+      <c r="C42" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="D42" s="5">
+      <c r="D42" s="5" t="n">
         <v>3</v>
       </c>
       <c r="E42" s="5"/>
@@ -2757,20 +1646,20 @@
       <c r="N42" s="5"/>
       <c r="O42" s="5"/>
     </row>
-    <row r="43" ht="20.35" customHeight="1">
-      <c r="A43" t="s" s="2">
+    <row r="43" customFormat="false" ht="20.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A43" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B43" s="3">
+      <c r="B43" s="3" t="n">
         <v>43</v>
       </c>
-      <c r="C43" t="s" s="4">
+      <c r="C43" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="D43" s="5">
+      <c r="D43" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="E43" s="5">
+      <c r="E43" s="5" t="n">
         <v>5</v>
       </c>
       <c r="F43" s="5"/>
@@ -2784,20 +1673,20 @@
       <c r="N43" s="5"/>
       <c r="O43" s="5"/>
     </row>
-    <row r="44" ht="20.35" customHeight="1">
-      <c r="A44" t="s" s="2">
+    <row r="44" customFormat="false" ht="20.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A44" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B44" s="3">
+      <c r="B44" s="3" t="n">
         <v>44</v>
       </c>
-      <c r="C44" t="s" s="4">
+      <c r="C44" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="D44" s="5">
+      <c r="D44" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="E44" s="5">
+      <c r="E44" s="5" t="n">
         <v>5</v>
       </c>
       <c r="F44" s="5"/>
@@ -2811,29 +1700,29 @@
       <c r="N44" s="5"/>
       <c r="O44" s="5"/>
     </row>
-    <row r="45" ht="20.35" customHeight="1">
-      <c r="A45" t="s" s="2">
+    <row r="45" customFormat="false" ht="20.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A45" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B45" s="3">
+      <c r="B45" s="3" t="n">
         <v>45</v>
       </c>
-      <c r="C45" t="s" s="4">
+      <c r="C45" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="D45" s="5">
+      <c r="D45" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="E45" s="5">
+      <c r="E45" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="F45" s="5">
+      <c r="F45" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="G45" t="s" s="6">
+      <c r="G45" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="H45" t="s" s="6">
+      <c r="H45" s="6" t="s">
         <v>51</v>
       </c>
       <c r="I45" s="5"/>
@@ -2844,106 +1733,106 @@
       <c r="N45" s="5"/>
       <c r="O45" s="5"/>
     </row>
-    <row r="46" ht="20.35" customHeight="1">
-      <c r="A46" t="s" s="2">
+    <row r="46" customFormat="false" ht="20.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A46" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B46" s="3">
+      <c r="B46" s="3" t="n">
         <v>46</v>
       </c>
-      <c r="C46" t="s" s="4">
+      <c r="C46" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="D46" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="E46" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="F46" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="D46" s="5">
-        <v>6</v>
-      </c>
-      <c r="E46" t="s" s="6">
-        <v>50</v>
-      </c>
-      <c r="F46" t="s" s="6">
+      <c r="G46" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H46" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="G46" t="s" s="6">
+      <c r="I46" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="H46" t="s" s="6">
+      <c r="J46" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="I46" t="s" s="6">
-        <v>51</v>
-      </c>
-      <c r="J46" s="5"/>
-      <c r="K46" s="5"/>
+      <c r="K46" s="6" t="s">
+        <v>24</v>
+      </c>
       <c r="L46" s="5"/>
       <c r="M46" s="5"/>
       <c r="N46" s="5"/>
       <c r="O46" s="5"/>
     </row>
-    <row r="47" ht="20.35" customHeight="1">
-      <c r="A47" t="s" s="2">
+    <row r="47" customFormat="false" ht="20.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A47" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B47" s="3">
+      <c r="B47" s="3" t="n">
         <v>47</v>
       </c>
-      <c r="C47" t="s" s="4">
-        <v>61</v>
-      </c>
-      <c r="D47" s="5">
+      <c r="C47" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D47" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="E47" s="5">
+      <c r="E47" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="F47" s="5">
+      <c r="F47" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="G47" t="s" s="6">
-        <v>11</v>
-      </c>
-      <c r="H47" t="s" s="6">
-        <v>21</v>
-      </c>
-      <c r="I47" t="s" s="6">
-        <v>22</v>
-      </c>
-      <c r="J47" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="K47" t="s" s="6">
-        <v>24</v>
-      </c>
+      <c r="G47" s="5" t="n">
+        <v>7</v>
+      </c>
+      <c r="H47" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="I47" s="5"/>
+      <c r="J47" s="5"/>
+      <c r="K47" s="5"/>
       <c r="L47" s="5"/>
       <c r="M47" s="5"/>
       <c r="N47" s="5"/>
       <c r="O47" s="5"/>
     </row>
-    <row r="48" ht="20.35" customHeight="1">
-      <c r="A48" t="s" s="2">
+    <row r="48" customFormat="false" ht="20.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A48" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B48" s="3">
+      <c r="B48" s="3" t="n">
         <v>48</v>
       </c>
-      <c r="C48" t="s" s="4">
-        <v>62</v>
-      </c>
-      <c r="D48" s="5">
+      <c r="C48" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D48" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="E48" s="5">
+      <c r="E48" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="F48" s="5">
+      <c r="F48" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="G48" s="5">
-        <v>7</v>
-      </c>
-      <c r="H48" t="s" s="6">
-        <v>23</v>
-      </c>
-      <c r="I48" s="5"/>
+      <c r="G48" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="H48" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="I48" s="6" t="s">
+        <v>24</v>
+      </c>
       <c r="J48" s="5"/>
       <c r="K48" s="5"/>
       <c r="L48" s="5"/>
@@ -2951,34 +1840,28 @@
       <c r="N48" s="5"/>
       <c r="O48" s="5"/>
     </row>
-    <row r="49" ht="20.35" customHeight="1">
-      <c r="A49" t="s" s="2">
+    <row r="49" customFormat="false" ht="20.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A49" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B49" s="3">
+      <c r="B49" s="3" t="n">
         <v>49</v>
       </c>
-      <c r="C49" t="s" s="4">
-        <v>63</v>
-      </c>
-      <c r="D49" s="5">
+      <c r="C49" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D49" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="E49" s="5">
+      <c r="E49" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="F49" s="5">
+      <c r="F49" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="G49" t="s" s="6">
-        <v>21</v>
-      </c>
-      <c r="H49" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="I49" t="s" s="6">
-        <v>24</v>
-      </c>
+      <c r="G49" s="5"/>
+      <c r="H49" s="5"/>
+      <c r="I49" s="5"/>
       <c r="J49" s="5"/>
       <c r="K49" s="5"/>
       <c r="L49" s="5"/>
@@ -2986,23 +1869,23 @@
       <c r="N49" s="5"/>
       <c r="O49" s="5"/>
     </row>
-    <row r="50" ht="20.35" customHeight="1">
-      <c r="A50" t="s" s="2">
+    <row r="50" customFormat="false" ht="20.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A50" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B50" s="3">
+      <c r="B50" s="3" t="n">
         <v>50</v>
       </c>
-      <c r="C50" t="s" s="4">
-        <v>32</v>
-      </c>
-      <c r="D50" s="5">
+      <c r="C50" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D50" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="E50" s="5">
+      <c r="E50" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="F50" s="5">
+      <c r="F50" s="5" t="n">
         <v>6</v>
       </c>
       <c r="G50" s="5"/>
@@ -3015,28 +1898,34 @@
       <c r="N50" s="5"/>
       <c r="O50" s="5"/>
     </row>
-    <row r="51" ht="20.35" customHeight="1">
-      <c r="A51" t="s" s="2">
+    <row r="51" customFormat="false" ht="20.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A51" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B51" s="3">
+      <c r="B51" s="3" t="n">
         <v>51</v>
       </c>
-      <c r="C51" t="s" s="4">
-        <v>37</v>
-      </c>
-      <c r="D51" s="5">
-        <v>4</v>
-      </c>
-      <c r="E51" s="5">
-        <v>5</v>
-      </c>
-      <c r="F51" s="5">
+      <c r="C51" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G51" s="5"/>
-      <c r="H51" s="5"/>
-      <c r="I51" s="5"/>
+      <c r="D51" s="5" t="n">
+        <v>6</v>
+      </c>
+      <c r="E51" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="F51" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G51" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="H51" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="I51" s="6" t="s">
+        <v>51</v>
+      </c>
       <c r="J51" s="5"/>
       <c r="K51" s="5"/>
       <c r="L51" s="5"/>
@@ -3044,17 +1933,17 @@
       <c r="N51" s="5"/>
       <c r="O51" s="5"/>
     </row>
-    <row r="52" ht="20.35" customHeight="1">
-      <c r="A52" t="s" s="2">
+    <row r="52" customFormat="false" ht="20.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A52" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B52" s="3">
+      <c r="B52" s="3" t="n">
         <v>52</v>
       </c>
-      <c r="C52" t="s" s="4">
+      <c r="C52" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="D52" s="5">
+      <c r="D52" s="5" t="n">
         <v>6</v>
       </c>
       <c r="E52" s="5"/>
@@ -3069,29 +1958,29 @@
       <c r="N52" s="5"/>
       <c r="O52" s="5"/>
     </row>
-    <row r="53" ht="20.35" customHeight="1">
-      <c r="A53" t="s" s="2">
+    <row r="53" customFormat="false" ht="20.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A53" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B53" s="3">
+      <c r="B53" s="3" t="n">
         <v>53</v>
       </c>
-      <c r="C53" t="s" s="4">
+      <c r="C53" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="D53" s="5">
+      <c r="D53" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="E53" t="s" s="6">
+      <c r="E53" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="F53" t="s" s="6">
+      <c r="F53" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="G53" t="s" s="6">
+      <c r="G53" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="H53" t="s" s="6">
+      <c r="H53" s="6" t="s">
         <v>12</v>
       </c>
       <c r="I53" s="5"/>
@@ -3102,17 +1991,17 @@
       <c r="N53" s="5"/>
       <c r="O53" s="5"/>
     </row>
-    <row r="54" ht="20.35" customHeight="1">
-      <c r="A54" t="s" s="2">
+    <row r="54" customFormat="false" ht="20.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A54" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B54" s="3">
+      <c r="B54" s="3" t="n">
         <v>54</v>
       </c>
-      <c r="C54" t="s" s="4">
+      <c r="C54" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="D54" s="5">
+      <c r="D54" s="5" t="n">
         <v>6</v>
       </c>
       <c r="E54" s="5"/>
@@ -3127,17 +2016,17 @@
       <c r="N54" s="5"/>
       <c r="O54" s="5"/>
     </row>
-    <row r="55" ht="20.35" customHeight="1">
-      <c r="A55" t="s" s="2">
+    <row r="55" customFormat="false" ht="20.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A55" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B55" s="3">
+      <c r="B55" s="3" t="n">
         <v>55</v>
       </c>
-      <c r="C55" t="s" s="4">
+      <c r="C55" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D55" s="5">
+      <c r="D55" s="5" t="n">
         <v>6</v>
       </c>
       <c r="E55" s="5"/>
@@ -3152,17 +2041,17 @@
       <c r="N55" s="5"/>
       <c r="O55" s="5"/>
     </row>
-    <row r="56" ht="20.35" customHeight="1">
-      <c r="A56" t="s" s="2">
+    <row r="56" customFormat="false" ht="20.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A56" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B56" s="3">
+      <c r="B56" s="3" t="n">
         <v>56</v>
       </c>
-      <c r="C56" t="s" s="4">
+      <c r="C56" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D56" s="5">
+      <c r="D56" s="5" t="n">
         <v>6</v>
       </c>
       <c r="E56" s="5"/>
@@ -3177,17 +2066,17 @@
       <c r="N56" s="5"/>
       <c r="O56" s="5"/>
     </row>
-    <row r="57" ht="20.35" customHeight="1">
-      <c r="A57" t="s" s="2">
+    <row r="57" customFormat="false" ht="20.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A57" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B57" s="3">
+      <c r="B57" s="3" t="n">
         <v>57</v>
       </c>
-      <c r="C57" t="s" s="4">
+      <c r="C57" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="D57" s="5">
+      <c r="D57" s="5" t="n">
         <v>6</v>
       </c>
       <c r="E57" s="5"/>
@@ -3202,23 +2091,23 @@
       <c r="N57" s="5"/>
       <c r="O57" s="5"/>
     </row>
-    <row r="58" ht="20.35" customHeight="1">
-      <c r="A58" t="s" s="2">
+    <row r="58" customFormat="false" ht="20.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A58" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B58" s="3">
+      <c r="B58" s="3" t="n">
         <v>58</v>
       </c>
-      <c r="C58" t="s" s="4">
+      <c r="C58" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="D58" s="5">
+      <c r="D58" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="E58" t="s" s="6">
+      <c r="E58" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="F58" t="s" s="6">
+      <c r="F58" s="6" t="s">
         <v>12</v>
       </c>
       <c r="G58" s="5"/>
@@ -3231,17 +2120,17 @@
       <c r="N58" s="5"/>
       <c r="O58" s="5"/>
     </row>
-    <row r="59" ht="20.35" customHeight="1">
-      <c r="A59" t="s" s="2">
+    <row r="59" customFormat="false" ht="20.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A59" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B59" s="3">
+      <c r="B59" s="3" t="n">
         <v>59</v>
       </c>
-      <c r="C59" t="s" s="4">
+      <c r="C59" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="D59" s="5">
+      <c r="D59" s="5" t="n">
         <v>6</v>
       </c>
       <c r="E59" s="5"/>
@@ -3256,17 +2145,17 @@
       <c r="N59" s="5"/>
       <c r="O59" s="5"/>
     </row>
-    <row r="60" ht="20.35" customHeight="1">
-      <c r="A60" t="s" s="2">
+    <row r="60" customFormat="false" ht="20.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A60" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B60" s="3">
+      <c r="B60" s="3" t="n">
         <v>60</v>
       </c>
-      <c r="C60" t="s" s="4">
+      <c r="C60" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="D60" s="5">
+      <c r="D60" s="5" t="n">
         <v>6</v>
       </c>
       <c r="E60" s="5"/>
@@ -3281,17 +2170,17 @@
       <c r="N60" s="5"/>
       <c r="O60" s="5"/>
     </row>
-    <row r="61" ht="20.35" customHeight="1">
-      <c r="A61" t="s" s="2">
+    <row r="61" customFormat="false" ht="20.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A61" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B61" s="3">
+      <c r="B61" s="3" t="n">
         <v>61</v>
       </c>
-      <c r="C61" t="s" s="4">
+      <c r="C61" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="D61" s="5">
+      <c r="D61" s="5" t="n">
         <v>6</v>
       </c>
       <c r="E61" s="5"/>
@@ -3306,17 +2195,17 @@
       <c r="N61" s="5"/>
       <c r="O61" s="5"/>
     </row>
-    <row r="62" ht="20.35" customHeight="1">
-      <c r="A62" t="s" s="2">
+    <row r="62" customFormat="false" ht="20.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A62" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B62" s="3">
+      <c r="B62" s="3" t="n">
         <v>62</v>
       </c>
-      <c r="C62" t="s" s="4">
+      <c r="C62" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="D62" s="5">
+      <c r="D62" s="5" t="n">
         <v>6</v>
       </c>
       <c r="E62" s="5"/>
@@ -3331,17 +2220,17 @@
       <c r="N62" s="5"/>
       <c r="O62" s="5"/>
     </row>
-    <row r="63" ht="20.35" customHeight="1">
-      <c r="A63" t="s" s="2">
+    <row r="63" customFormat="false" ht="20.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A63" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B63" s="3">
+      <c r="B63" s="3" t="n">
         <v>63</v>
       </c>
-      <c r="C63" t="s" s="4">
+      <c r="C63" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="D63" s="5">
+      <c r="D63" s="5" t="n">
         <v>6</v>
       </c>
       <c r="E63" s="5"/>
@@ -3356,17 +2245,17 @@
       <c r="N63" s="5"/>
       <c r="O63" s="5"/>
     </row>
-    <row r="64" ht="20.35" customHeight="1">
-      <c r="A64" t="s" s="2">
+    <row r="64" customFormat="false" ht="20.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A64" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B64" s="3">
+      <c r="B64" s="3" t="n">
         <v>64</v>
       </c>
-      <c r="C64" t="s" s="4">
+      <c r="C64" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="D64" s="5">
+      <c r="D64" s="5" t="n">
         <v>6</v>
       </c>
       <c r="E64" s="5"/>
@@ -3381,17 +2270,17 @@
       <c r="N64" s="5"/>
       <c r="O64" s="5"/>
     </row>
-    <row r="65" ht="20.35" customHeight="1">
-      <c r="A65" t="s" s="2">
+    <row r="65" customFormat="false" ht="20.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A65" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="B65" s="3">
+      <c r="B65" s="3" t="n">
         <v>65</v>
       </c>
-      <c r="C65" t="s" s="4">
+      <c r="C65" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="D65" s="5">
+      <c r="D65" s="5" t="n">
         <v>7</v>
       </c>
       <c r="E65" s="5"/>
@@ -3406,29 +2295,29 @@
       <c r="N65" s="5"/>
       <c r="O65" s="5"/>
     </row>
-    <row r="66" ht="20.35" customHeight="1">
-      <c r="A66" t="s" s="2">
+    <row r="66" customFormat="false" ht="20.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A66" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="B66" s="3">
+      <c r="B66" s="3" t="n">
         <v>66</v>
       </c>
-      <c r="C66" t="s" s="4">
+      <c r="C66" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="D66" s="5">
+      <c r="D66" s="5" t="n">
         <v>7</v>
       </c>
-      <c r="E66" t="s" s="6">
+      <c r="E66" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="F66" t="s" s="6">
+      <c r="F66" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="G66" t="s" s="6">
+      <c r="G66" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="H66" t="s" s="6">
+      <c r="H66" s="6" t="s">
         <v>12</v>
       </c>
       <c r="I66" s="5"/>
@@ -3439,23 +2328,23 @@
       <c r="N66" s="5"/>
       <c r="O66" s="5"/>
     </row>
-    <row r="67" ht="20.35" customHeight="1">
-      <c r="A67" t="s" s="2">
+    <row r="67" customFormat="false" ht="20.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A67" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B67" s="3">
+      <c r="B67" s="3" t="n">
         <v>67</v>
       </c>
-      <c r="C67" t="s" s="4">
+      <c r="C67" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D67" t="s" s="6">
+      <c r="D67" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E67" t="s" s="6">
+      <c r="E67" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="F67" t="s" s="6">
+      <c r="F67" s="6" t="s">
         <v>20</v>
       </c>
       <c r="G67" s="5"/>
@@ -3468,35 +2357,35 @@
       <c r="N67" s="5"/>
       <c r="O67" s="5"/>
     </row>
-    <row r="68" ht="20.35" customHeight="1">
-      <c r="A68" t="s" s="2">
+    <row r="68" customFormat="false" ht="20.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A68" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B68" s="3">
+      <c r="B68" s="3" t="n">
         <v>68</v>
       </c>
-      <c r="C68" t="s" s="4">
+      <c r="C68" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="D68" t="s" s="6">
+      <c r="D68" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E68" t="s" s="6">
+      <c r="E68" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="F68" t="s" s="6">
+      <c r="F68" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="G68" t="s" s="6">
+      <c r="G68" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="H68" t="s" s="6">
+      <c r="H68" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="I68" t="s" s="6">
+      <c r="I68" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="J68" t="s" s="6">
+      <c r="J68" s="6" t="s">
         <v>12</v>
       </c>
       <c r="K68" s="5"/>
@@ -3505,26 +2394,26 @@
       <c r="N68" s="5"/>
       <c r="O68" s="5"/>
     </row>
-    <row r="69" ht="20.35" customHeight="1">
-      <c r="A69" t="s" s="2">
+    <row r="69" customFormat="false" ht="20.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A69" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B69" s="3">
+      <c r="B69" s="3" t="n">
         <v>69</v>
       </c>
-      <c r="C69" t="s" s="4">
+      <c r="C69" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D69" t="s" s="6">
+      <c r="D69" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E69" t="s" s="6">
+      <c r="E69" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="F69" t="s" s="6">
+      <c r="F69" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="G69" t="s" s="6">
+      <c r="G69" s="6" t="s">
         <v>11</v>
       </c>
       <c r="H69" s="5"/>
@@ -3536,23 +2425,23 @@
       <c r="N69" s="5"/>
       <c r="O69" s="5"/>
     </row>
-    <row r="70" ht="20.35" customHeight="1">
-      <c r="A70" t="s" s="2">
+    <row r="70" customFormat="false" ht="20.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A70" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B70" s="3">
+      <c r="B70" s="3" t="n">
         <v>70</v>
       </c>
-      <c r="C70" t="s" s="4">
+      <c r="C70" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D70" t="s" s="6">
+      <c r="D70" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E70" t="s" s="6">
+      <c r="E70" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="F70" t="s" s="6">
+      <c r="F70" s="6" t="s">
         <v>20</v>
       </c>
       <c r="G70" s="5"/>
@@ -3565,26 +2454,26 @@
       <c r="N70" s="5"/>
       <c r="O70" s="5"/>
     </row>
-    <row r="71" ht="20.35" customHeight="1">
-      <c r="A71" t="s" s="2">
+    <row r="71" customFormat="false" ht="20.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A71" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B71" s="3">
+      <c r="B71" s="3" t="n">
         <v>71</v>
       </c>
-      <c r="C71" t="s" s="4">
+      <c r="C71" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="D71" t="s" s="6">
+      <c r="D71" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E71" t="s" s="6">
+      <c r="E71" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="F71" t="s" s="6">
+      <c r="F71" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="G71" t="s" s="6">
+      <c r="G71" s="6" t="s">
         <v>28</v>
       </c>
       <c r="H71" s="5"/>
@@ -3596,26 +2485,26 @@
       <c r="N71" s="5"/>
       <c r="O71" s="5"/>
     </row>
-    <row r="72" ht="20.35" customHeight="1">
-      <c r="A72" t="s" s="2">
+    <row r="72" customFormat="false" ht="20.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A72" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B72" s="3">
+      <c r="B72" s="3" t="n">
         <v>72</v>
       </c>
-      <c r="C72" t="s" s="4">
+      <c r="C72" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="D72" t="s" s="6">
+      <c r="D72" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E72" t="s" s="6">
+      <c r="E72" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="F72" t="s" s="6">
+      <c r="F72" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="G72" t="s" s="6">
+      <c r="G72" s="6" t="s">
         <v>28</v>
       </c>
       <c r="H72" s="5"/>
@@ -3627,20 +2516,20 @@
       <c r="N72" s="5"/>
       <c r="O72" s="5"/>
     </row>
-    <row r="73" ht="20.35" customHeight="1">
-      <c r="A73" t="s" s="2">
+    <row r="73" customFormat="false" ht="20.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A73" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B73" s="3">
+      <c r="B73" s="3" t="n">
         <v>73</v>
       </c>
-      <c r="C73" t="s" s="4">
+      <c r="C73" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="D73" t="s" s="6">
+      <c r="D73" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E73" t="s" s="6">
+      <c r="E73" s="6" t="s">
         <v>19</v>
       </c>
       <c r="F73" s="5"/>
@@ -3654,17 +2543,17 @@
       <c r="N73" s="5"/>
       <c r="O73" s="5"/>
     </row>
-    <row r="74" ht="20.35" customHeight="1">
-      <c r="A74" t="s" s="2">
+    <row r="74" customFormat="false" ht="20.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A74" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B74" s="3">
+      <c r="B74" s="3" t="n">
         <v>74</v>
       </c>
-      <c r="C74" t="s" s="4">
+      <c r="C74" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="D74" t="s" s="6">
+      <c r="D74" s="6" t="s">
         <v>18</v>
       </c>
       <c r="E74" s="5"/>
@@ -3679,17 +2568,17 @@
       <c r="N74" s="5"/>
       <c r="O74" s="5"/>
     </row>
-    <row r="75" ht="20.35" customHeight="1">
-      <c r="A75" t="s" s="2">
+    <row r="75" customFormat="false" ht="20.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A75" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B75" s="3">
+      <c r="B75" s="3" t="n">
         <v>75</v>
       </c>
-      <c r="C75" t="s" s="4">
+      <c r="C75" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="D75" t="s" s="6">
+      <c r="D75" s="6" t="s">
         <v>18</v>
       </c>
       <c r="E75" s="5"/>
@@ -3704,17 +2593,17 @@
       <c r="N75" s="5"/>
       <c r="O75" s="5"/>
     </row>
-    <row r="76" ht="20.35" customHeight="1">
-      <c r="A76" t="s" s="2">
+    <row r="76" customFormat="false" ht="20.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A76" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B76" s="3">
+      <c r="B76" s="3" t="n">
         <v>76</v>
       </c>
-      <c r="C76" t="s" s="4">
+      <c r="C76" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="D76" t="s" s="6">
+      <c r="D76" s="6" t="s">
         <v>18</v>
       </c>
       <c r="E76" s="5"/>
@@ -3729,17 +2618,17 @@
       <c r="N76" s="5"/>
       <c r="O76" s="5"/>
     </row>
-    <row r="77" ht="20.35" customHeight="1">
-      <c r="A77" t="s" s="2">
+    <row r="77" customFormat="false" ht="20.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A77" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B77" s="3">
+      <c r="B77" s="3" t="n">
         <v>77</v>
       </c>
-      <c r="C77" t="s" s="4">
+      <c r="C77" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="D77" t="s" s="6">
+      <c r="D77" s="6" t="s">
         <v>18</v>
       </c>
       <c r="E77" s="5"/>
@@ -3754,17 +2643,17 @@
       <c r="N77" s="5"/>
       <c r="O77" s="5"/>
     </row>
-    <row r="78" ht="20.35" customHeight="1">
-      <c r="A78" t="s" s="2">
+    <row r="78" customFormat="false" ht="20.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A78" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B78" s="3">
+      <c r="B78" s="3" t="n">
         <v>78</v>
       </c>
-      <c r="C78" t="s" s="4">
+      <c r="C78" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="D78" t="s" s="6">
+      <c r="D78" s="6" t="s">
         <v>18</v>
       </c>
       <c r="E78" s="5"/>
@@ -3779,20 +2668,20 @@
       <c r="N78" s="5"/>
       <c r="O78" s="5"/>
     </row>
-    <row r="79" ht="20.35" customHeight="1">
-      <c r="A79" t="s" s="2">
+    <row r="79" customFormat="false" ht="20.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A79" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="B79" s="3">
+      <c r="B79" s="3" t="n">
         <v>79</v>
       </c>
-      <c r="C79" t="s" s="4">
+      <c r="C79" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="D79" t="s" s="6">
+      <c r="D79" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="E79" t="s" s="6">
+      <c r="E79" s="6" t="s">
         <v>28</v>
       </c>
       <c r="F79" s="6"/>
@@ -3806,35 +2695,35 @@
       <c r="N79" s="5"/>
       <c r="O79" s="5"/>
     </row>
-    <row r="80" ht="20.35" customHeight="1">
-      <c r="A80" t="s" s="2">
+    <row r="80" customFormat="false" ht="20.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A80" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="B80" s="3">
+      <c r="B80" s="3" t="n">
         <v>80</v>
       </c>
-      <c r="C80" t="s" s="4">
+      <c r="C80" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="D80" t="s" s="6">
+      <c r="D80" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="E80" t="s" s="6">
+      <c r="E80" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="F80" t="s" s="6">
+      <c r="F80" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G80" t="s" s="6">
+      <c r="G80" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="H80" t="s" s="6">
+      <c r="H80" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="I80" t="s" s="6">
+      <c r="I80" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="J80" t="s" s="6">
+      <c r="J80" s="6" t="s">
         <v>2</v>
       </c>
       <c r="K80" s="5"/>
@@ -3843,26 +2732,26 @@
       <c r="N80" s="5"/>
       <c r="O80" s="5"/>
     </row>
-    <row r="81" ht="20.35" customHeight="1">
-      <c r="A81" t="s" s="2">
+    <row r="81" customFormat="false" ht="20.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A81" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="B81" s="3">
+      <c r="B81" s="3" t="n">
         <v>81</v>
       </c>
-      <c r="C81" t="s" s="4">
+      <c r="C81" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="D81" t="s" s="6">
+      <c r="D81" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="E81" t="s" s="6">
+      <c r="E81" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="F81" t="s" s="6">
+      <c r="F81" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G81" t="s" s="6">
+      <c r="G81" s="6" t="s">
         <v>12</v>
       </c>
       <c r="H81" s="5"/>
@@ -3874,23 +2763,23 @@
       <c r="N81" s="5"/>
       <c r="O81" s="5"/>
     </row>
-    <row r="82" ht="20.35" customHeight="1">
-      <c r="A82" t="s" s="2">
+    <row r="82" customFormat="false" ht="20.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A82" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="B82" s="3">
+      <c r="B82" s="3" t="n">
         <v>82</v>
       </c>
-      <c r="C82" t="s" s="4">
+      <c r="C82" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="D82" t="s" s="6">
+      <c r="D82" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="E82" t="s" s="6">
+      <c r="E82" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="F82" t="s" s="6">
+      <c r="F82" s="6" t="s">
         <v>20</v>
       </c>
       <c r="G82" s="5"/>
@@ -3903,20 +2792,20 @@
       <c r="N82" s="5"/>
       <c r="O82" s="5"/>
     </row>
-    <row r="83" ht="20.35" customHeight="1">
-      <c r="A83" t="s" s="2">
+    <row r="83" customFormat="false" ht="20.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A83" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B83" s="3">
+      <c r="B83" s="3" t="n">
         <v>83</v>
       </c>
-      <c r="C83" t="s" s="4">
+      <c r="C83" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="D83" t="s" s="6">
+      <c r="D83" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="E83" t="s" s="6">
+      <c r="E83" s="6" t="s">
         <v>19</v>
       </c>
       <c r="F83" s="5"/>
@@ -3930,20 +2819,20 @@
       <c r="N83" s="5"/>
       <c r="O83" s="5"/>
     </row>
-    <row r="84" ht="20.35" customHeight="1">
-      <c r="A84" t="s" s="2">
+    <row r="84" customFormat="false" ht="20.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A84" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B84" s="3">
+      <c r="B84" s="3" t="n">
         <v>84</v>
       </c>
-      <c r="C84" t="s" s="4">
+      <c r="C84" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="D84" t="s" s="6">
+      <c r="D84" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="E84" t="s" s="6">
+      <c r="E84" s="6" t="s">
         <v>19</v>
       </c>
       <c r="F84" s="5"/>
@@ -3957,20 +2846,20 @@
       <c r="N84" s="5"/>
       <c r="O84" s="5"/>
     </row>
-    <row r="85" ht="20.35" customHeight="1">
-      <c r="A85" t="s" s="2">
+    <row r="85" customFormat="false" ht="20.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A85" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B85" s="3">
+      <c r="B85" s="3" t="n">
         <v>85</v>
       </c>
-      <c r="C85" t="s" s="4">
+      <c r="C85" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D85" t="s" s="6">
+      <c r="D85" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="E85" t="s" s="6">
+      <c r="E85" s="6" t="s">
         <v>19</v>
       </c>
       <c r="F85" s="5"/>
@@ -3984,20 +2873,20 @@
       <c r="N85" s="5"/>
       <c r="O85" s="5"/>
     </row>
-    <row r="86" ht="20.35" customHeight="1">
-      <c r="A86" t="s" s="2">
+    <row r="86" customFormat="false" ht="20.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A86" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B86" s="3">
+      <c r="B86" s="3" t="n">
         <v>86</v>
       </c>
-      <c r="C86" t="s" s="4">
+      <c r="C86" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="D86" t="s" s="6">
+      <c r="D86" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="E86" t="s" s="6">
+      <c r="E86" s="6" t="s">
         <v>19</v>
       </c>
       <c r="F86" s="5"/>
@@ -4011,20 +2900,20 @@
       <c r="N86" s="5"/>
       <c r="O86" s="5"/>
     </row>
-    <row r="87" ht="20.35" customHeight="1">
-      <c r="A87" t="s" s="2">
+    <row r="87" customFormat="false" ht="20.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A87" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B87" s="3">
+      <c r="B87" s="3" t="n">
         <v>87</v>
       </c>
-      <c r="C87" t="s" s="4">
+      <c r="C87" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="D87" t="s" s="6">
+      <c r="D87" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="E87" t="s" s="6">
+      <c r="E87" s="6" t="s">
         <v>19</v>
       </c>
       <c r="F87" s="5"/>
@@ -4038,20 +2927,20 @@
       <c r="N87" s="5"/>
       <c r="O87" s="5"/>
     </row>
-    <row r="88" ht="20.35" customHeight="1">
-      <c r="A88" t="s" s="2">
+    <row r="88" customFormat="false" ht="20.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A88" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B88" s="3">
+      <c r="B88" s="3" t="n">
         <v>88</v>
       </c>
-      <c r="C88" t="s" s="4">
+      <c r="C88" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D88" t="s" s="6">
+      <c r="D88" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="E88" t="s" s="6">
+      <c r="E88" s="6" t="s">
         <v>19</v>
       </c>
       <c r="F88" s="5"/>
@@ -4065,20 +2954,20 @@
       <c r="N88" s="5"/>
       <c r="O88" s="5"/>
     </row>
-    <row r="89" ht="20.35" customHeight="1">
-      <c r="A89" t="s" s="2">
+    <row r="89" customFormat="false" ht="20.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A89" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B89" s="3">
+      <c r="B89" s="3" t="n">
         <v>89</v>
       </c>
-      <c r="C89" t="s" s="4">
+      <c r="C89" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="D89" t="s" s="6">
+      <c r="D89" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="E89" t="s" s="6">
+      <c r="E89" s="6" t="s">
         <v>19</v>
       </c>
       <c r="F89" s="5"/>
@@ -4092,20 +2981,20 @@
       <c r="N89" s="5"/>
       <c r="O89" s="5"/>
     </row>
-    <row r="90" ht="20.35" customHeight="1">
-      <c r="A90" t="s" s="2">
+    <row r="90" customFormat="false" ht="20.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A90" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B90" s="3">
+      <c r="B90" s="3" t="n">
         <v>90</v>
       </c>
-      <c r="C90" t="s" s="4">
+      <c r="C90" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="D90" t="s" s="6">
+      <c r="D90" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="E90" t="s" s="6">
+      <c r="E90" s="6" t="s">
         <v>19</v>
       </c>
       <c r="F90" s="5"/>
@@ -4119,20 +3008,20 @@
       <c r="N90" s="5"/>
       <c r="O90" s="5"/>
     </row>
-    <row r="91" ht="20.35" customHeight="1">
-      <c r="A91" t="s" s="2">
+    <row r="91" customFormat="false" ht="20.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A91" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B91" s="3">
+      <c r="B91" s="3" t="n">
         <v>91</v>
       </c>
-      <c r="C91" t="s" s="4">
+      <c r="C91" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="D91" t="s" s="6">
+      <c r="D91" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="E91" t="s" s="6">
+      <c r="E91" s="6" t="s">
         <v>28</v>
       </c>
       <c r="F91" s="5"/>
@@ -4146,20 +3035,20 @@
       <c r="N91" s="5"/>
       <c r="O91" s="5"/>
     </row>
-    <row r="92" ht="20.35" customHeight="1">
-      <c r="A92" t="s" s="2">
+    <row r="92" customFormat="false" ht="20.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A92" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B92" s="3">
+      <c r="B92" s="3" t="n">
         <v>92</v>
       </c>
-      <c r="C92" t="s" s="4">
+      <c r="C92" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="D92" t="s" s="6">
+      <c r="D92" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="E92" t="s" s="6">
+      <c r="E92" s="6" t="s">
         <v>20</v>
       </c>
       <c r="F92" s="5"/>
@@ -4173,20 +3062,20 @@
       <c r="N92" s="5"/>
       <c r="O92" s="5"/>
     </row>
-    <row r="93" ht="20.35" customHeight="1">
-      <c r="A93" t="s" s="2">
+    <row r="93" customFormat="false" ht="20.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A93" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B93" s="3">
+      <c r="B93" s="3" t="n">
         <v>93</v>
       </c>
-      <c r="C93" t="s" s="4">
+      <c r="C93" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D93" t="s" s="6">
+      <c r="D93" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="E93" t="s" s="6">
+      <c r="E93" s="6" t="s">
         <v>20</v>
       </c>
       <c r="F93" s="5"/>
@@ -4200,20 +3089,20 @@
       <c r="N93" s="5"/>
       <c r="O93" s="5"/>
     </row>
-    <row r="94" ht="20.35" customHeight="1">
-      <c r="A94" t="s" s="2">
+    <row r="94" customFormat="false" ht="20.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A94" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B94" s="3">
+      <c r="B94" s="3" t="n">
         <v>94</v>
       </c>
-      <c r="C94" t="s" s="4">
+      <c r="C94" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D94" t="s" s="6">
+      <c r="D94" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="E94" t="s" s="6">
+      <c r="E94" s="6" t="s">
         <v>20</v>
       </c>
       <c r="F94" s="5"/>
@@ -4227,17 +3116,17 @@
       <c r="N94" s="5"/>
       <c r="O94" s="5"/>
     </row>
-    <row r="95" ht="20.35" customHeight="1">
-      <c r="A95" t="s" s="2">
+    <row r="95" customFormat="false" ht="20.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A95" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B95" s="3">
+      <c r="B95" s="3" t="n">
         <v>95</v>
       </c>
-      <c r="C95" t="s" s="4">
+      <c r="C95" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="D95" t="s" s="6">
+      <c r="D95" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E95" s="5"/>
@@ -4252,17 +3141,17 @@
       <c r="N95" s="5"/>
       <c r="O95" s="5"/>
     </row>
-    <row r="96" ht="20.35" customHeight="1">
-      <c r="A96" t="s" s="2">
+    <row r="96" customFormat="false" ht="20.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A96" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B96" s="3">
+      <c r="B96" s="3" t="n">
         <v>96</v>
       </c>
-      <c r="C96" t="s" s="4">
+      <c r="C96" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="D96" t="s" s="6">
+      <c r="D96" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E96" s="5"/>
@@ -4277,20 +3166,20 @@
       <c r="N96" s="5"/>
       <c r="O96" s="5"/>
     </row>
-    <row r="97" ht="20.35" customHeight="1">
-      <c r="A97" t="s" s="2">
+    <row r="97" customFormat="false" ht="20.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A97" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="B97" s="3">
+      <c r="B97" s="3" t="n">
         <v>97</v>
       </c>
-      <c r="C97" t="s" s="4">
+      <c r="C97" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="D97" t="s" s="6">
+      <c r="D97" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E97" t="s" s="6">
+      <c r="E97" s="6" t="s">
         <v>12</v>
       </c>
       <c r="F97" s="5"/>
@@ -4304,17 +3193,17 @@
       <c r="N97" s="5"/>
       <c r="O97" s="5"/>
     </row>
-    <row r="98" ht="20.35" customHeight="1">
-      <c r="A98" t="s" s="2">
+    <row r="98" customFormat="false" ht="20.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A98" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="B98" s="3">
+      <c r="B98" s="3" t="n">
         <v>98</v>
       </c>
-      <c r="C98" t="s" s="4">
+      <c r="C98" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="D98" t="s" s="6">
+      <c r="D98" s="6" t="s">
         <v>10</v>
       </c>
       <c r="E98" s="5"/>
@@ -4329,26 +3218,26 @@
       <c r="N98" s="5"/>
       <c r="O98" s="5"/>
     </row>
-    <row r="99" ht="20.35" customHeight="1">
-      <c r="A99" t="s" s="2">
+    <row r="99" customFormat="false" ht="20.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A99" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="B99" s="3">
+      <c r="B99" s="3" t="n">
         <v>99</v>
       </c>
-      <c r="C99" t="s" s="4">
+      <c r="C99" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="D99" t="s" s="6">
+      <c r="D99" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E99" t="s" s="6">
+      <c r="E99" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="F99" t="s" s="6">
+      <c r="F99" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G99" t="s" s="6">
+      <c r="G99" s="6" t="s">
         <v>51</v>
       </c>
       <c r="H99" s="5"/>
@@ -4360,17 +3249,17 @@
       <c r="N99" s="5"/>
       <c r="O99" s="5"/>
     </row>
-    <row r="100" ht="20.35" customHeight="1">
-      <c r="A100" t="s" s="2">
+    <row r="100" customFormat="false" ht="20.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A100" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="B100" s="3">
+      <c r="B100" s="3" t="n">
         <v>100</v>
       </c>
-      <c r="C100" t="s" s="4">
+      <c r="C100" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="D100" t="s" s="6">
+      <c r="D100" s="6" t="s">
         <v>10</v>
       </c>
       <c r="E100" s="5"/>
@@ -4385,20 +3274,20 @@
       <c r="N100" s="5"/>
       <c r="O100" s="5"/>
     </row>
-    <row r="101" ht="20.35" customHeight="1">
-      <c r="A101" t="s" s="2">
+    <row r="101" customFormat="false" ht="20.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A101" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="B101" s="3">
+      <c r="B101" s="3" t="n">
         <v>101</v>
       </c>
-      <c r="C101" t="s" s="4">
+      <c r="C101" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D101" t="s" s="6">
+      <c r="D101" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E101" t="s" s="6">
+      <c r="E101" s="6" t="s">
         <v>12</v>
       </c>
       <c r="F101" s="5"/>
@@ -4412,20 +3301,20 @@
       <c r="N101" s="5"/>
       <c r="O101" s="5"/>
     </row>
-    <row r="102" ht="20.35" customHeight="1">
-      <c r="A102" t="s" s="2">
+    <row r="102" customFormat="false" ht="20.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A102" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="B102" s="3">
+      <c r="B102" s="3" t="n">
         <v>102</v>
       </c>
-      <c r="C102" t="s" s="4">
+      <c r="C102" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="D102" t="s" s="6">
+      <c r="D102" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E102" t="s" s="6">
+      <c r="E102" s="6" t="s">
         <v>22</v>
       </c>
       <c r="F102" s="5"/>
@@ -4439,23 +3328,23 @@
       <c r="N102" s="5"/>
       <c r="O102" s="5"/>
     </row>
-    <row r="103" ht="20.35" customHeight="1">
-      <c r="A103" t="s" s="2">
+    <row r="103" customFormat="false" ht="20.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A103" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="B103" s="3">
+      <c r="B103" s="3" t="n">
         <v>103</v>
       </c>
-      <c r="C103" t="s" s="4">
+      <c r="C103" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="D103" t="s" s="6">
+      <c r="D103" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E103" t="s" s="6">
+      <c r="E103" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="F103" t="s" s="6">
+      <c r="F103" s="6" t="s">
         <v>24</v>
       </c>
       <c r="G103" s="5"/>
@@ -4468,26 +3357,26 @@
       <c r="N103" s="5"/>
       <c r="O103" s="5"/>
     </row>
-    <row r="104" ht="20.35" customHeight="1">
-      <c r="A104" t="s" s="2">
+    <row r="104" customFormat="false" ht="20.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A104" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="B104" s="3">
+      <c r="B104" s="3" t="n">
         <v>104</v>
       </c>
-      <c r="C104" t="s" s="4">
+      <c r="C104" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="D104" t="s" s="6">
+      <c r="D104" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E104" t="s" s="6">
+      <c r="E104" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="F104" t="s" s="6">
+      <c r="F104" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="G104" t="s" s="6">
+      <c r="G104" s="6" t="s">
         <v>24</v>
       </c>
       <c r="H104" s="5"/>
@@ -4499,23 +3388,23 @@
       <c r="N104" s="5"/>
       <c r="O104" s="5"/>
     </row>
-    <row r="105" ht="20.35" customHeight="1">
-      <c r="A105" t="s" s="2">
+    <row r="105" customFormat="false" ht="20.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A105" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="B105" s="3">
+      <c r="B105" s="3" t="n">
         <v>105</v>
       </c>
-      <c r="C105" t="s" s="4">
+      <c r="C105" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="D105" t="s" s="6">
+      <c r="D105" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E105" t="s" s="6">
+      <c r="E105" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="F105" t="s" s="6">
+      <c r="F105" s="6" t="s">
         <v>24</v>
       </c>
       <c r="G105" s="5"/>
@@ -4528,17 +3417,17 @@
       <c r="N105" s="5"/>
       <c r="O105" s="5"/>
     </row>
-    <row r="106" ht="20.35" customHeight="1">
-      <c r="A106" t="s" s="2">
+    <row r="106" customFormat="false" ht="20.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A106" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="B106" s="3">
+      <c r="B106" s="3" t="n">
         <v>106</v>
       </c>
-      <c r="C106" t="s" s="4">
+      <c r="C106" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="D106" t="s" s="6">
+      <c r="D106" s="6" t="s">
         <v>22</v>
       </c>
       <c r="E106" s="5"/>
@@ -4553,17 +3442,17 @@
       <c r="N106" s="5"/>
       <c r="O106" s="5"/>
     </row>
-    <row r="107" ht="20.35" customHeight="1">
-      <c r="A107" t="s" s="2">
+    <row r="107" customFormat="false" ht="20.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A107" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="B107" s="3">
+      <c r="B107" s="3" t="n">
         <v>107</v>
       </c>
-      <c r="C107" t="s" s="4">
+      <c r="C107" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="D107" t="s" s="6">
+      <c r="D107" s="6" t="s">
         <v>22</v>
       </c>
       <c r="E107" s="5"/>
@@ -4578,17 +3467,17 @@
       <c r="N107" s="5"/>
       <c r="O107" s="5"/>
     </row>
-    <row r="108" ht="20.35" customHeight="1">
-      <c r="A108" t="s" s="2">
+    <row r="108" customFormat="false" ht="20.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A108" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="B108" s="3">
+      <c r="B108" s="3" t="n">
         <v>108</v>
       </c>
-      <c r="C108" t="s" s="4">
+      <c r="C108" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="D108" t="s" s="6">
+      <c r="D108" s="6" t="s">
         <v>22</v>
       </c>
       <c r="E108" s="5"/>
@@ -4603,20 +3492,20 @@
       <c r="N108" s="5"/>
       <c r="O108" s="5"/>
     </row>
-    <row r="109" ht="20.35" customHeight="1">
-      <c r="A109" t="s" s="2">
+    <row r="109" customFormat="false" ht="20.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A109" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="B109" s="3">
+      <c r="B109" s="3" t="n">
         <v>109</v>
       </c>
-      <c r="C109" t="s" s="4">
+      <c r="C109" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D109" t="s" s="6">
+      <c r="D109" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E109" t="s" s="6">
+      <c r="E109" s="6" t="s">
         <v>24</v>
       </c>
       <c r="F109" s="5"/>
@@ -4630,20 +3519,20 @@
       <c r="N109" s="5"/>
       <c r="O109" s="5"/>
     </row>
-    <row r="110" ht="20.35" customHeight="1">
-      <c r="A110" t="s" s="2">
+    <row r="110" customFormat="false" ht="20.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A110" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="B110" s="3">
+      <c r="B110" s="3" t="n">
         <v>110</v>
       </c>
-      <c r="C110" t="s" s="4">
+      <c r="C110" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="D110" t="s" s="6">
+      <c r="D110" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E110" t="s" s="6">
+      <c r="E110" s="6" t="s">
         <v>24</v>
       </c>
       <c r="F110" s="5"/>
@@ -4657,20 +3546,20 @@
       <c r="N110" s="5"/>
       <c r="O110" s="5"/>
     </row>
-    <row r="111" ht="20.35" customHeight="1">
-      <c r="A111" t="s" s="2">
+    <row r="111" customFormat="false" ht="20.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A111" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="B111" s="3">
+      <c r="B111" s="3" t="n">
         <v>111</v>
       </c>
-      <c r="C111" t="s" s="4">
+      <c r="C111" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="D111" t="s" s="6">
+      <c r="D111" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E111" t="s" s="6">
+      <c r="E111" s="6" t="s">
         <v>24</v>
       </c>
       <c r="F111" s="5"/>
@@ -4684,20 +3573,20 @@
       <c r="N111" s="5"/>
       <c r="O111" s="5"/>
     </row>
-    <row r="112" ht="20.35" customHeight="1">
-      <c r="A112" t="s" s="2">
+    <row r="112" customFormat="false" ht="20.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A112" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="B112" s="3">
+      <c r="B112" s="3" t="n">
         <v>112</v>
       </c>
-      <c r="C112" t="s" s="4">
+      <c r="C112" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="D112" t="s" s="6">
+      <c r="D112" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E112" t="s" s="6">
+      <c r="E112" s="6" t="s">
         <v>24</v>
       </c>
       <c r="F112" s="5"/>
@@ -4711,20 +3600,20 @@
       <c r="N112" s="5"/>
       <c r="O112" s="5"/>
     </row>
-    <row r="113" ht="20.35" customHeight="1">
-      <c r="A113" t="s" s="2">
+    <row r="113" customFormat="false" ht="20.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A113" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="B113" s="3">
+      <c r="B113" s="3" t="n">
         <v>113</v>
       </c>
-      <c r="C113" t="s" s="4">
+      <c r="C113" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="D113" t="s" s="6">
+      <c r="D113" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E113" t="s" s="6">
+      <c r="E113" s="6" t="s">
         <v>24</v>
       </c>
       <c r="F113" s="5"/>
@@ -4738,20 +3627,20 @@
       <c r="N113" s="5"/>
       <c r="O113" s="5"/>
     </row>
-    <row r="114" ht="20.35" customHeight="1">
-      <c r="A114" t="s" s="2">
+    <row r="114" customFormat="false" ht="20.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A114" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="B114" s="3">
+      <c r="B114" s="3" t="n">
         <v>114</v>
       </c>
-      <c r="C114" t="s" s="4">
+      <c r="C114" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D114" t="s" s="6">
+      <c r="D114" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E114" t="s" s="6">
+      <c r="E114" s="6" t="s">
         <v>24</v>
       </c>
       <c r="F114" s="5"/>
@@ -4765,20 +3654,20 @@
       <c r="N114" s="5"/>
       <c r="O114" s="5"/>
     </row>
-    <row r="115" ht="20.35" customHeight="1">
-      <c r="A115" t="s" s="2">
+    <row r="115" customFormat="false" ht="20.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A115" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="B115" s="3">
+      <c r="B115" s="3" t="n">
         <v>115</v>
       </c>
-      <c r="C115" t="s" s="4">
+      <c r="C115" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D115" t="s" s="6">
+      <c r="D115" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E115" t="s" s="6">
+      <c r="E115" s="6" t="s">
         <v>24</v>
       </c>
       <c r="F115" s="5"/>
@@ -4793,10 +3682,12 @@
       <c r="O115" s="5"/>
     </row>
   </sheetData>
-  <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
-  <headerFooter>
-    <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="1" right="1" top="1" bottom="1" header="0.511805555555555" footer="0.25"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter>&amp;C&amp;12&amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added the J and Z lines.
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="877" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="113">
   <si>
     <t>Broadway-7th Ave</t>
   </si>
@@ -309,6 +309,15 @@
   </si>
   <si>
     <t>Lexington Av - 63 St</t>
+  </si>
+  <si>
+    <t>Nassau Street</t>
+  </si>
+  <si>
+    <t>Broad St</t>
+  </si>
+  <si>
+    <t>Bowery</t>
   </si>
   <si>
     <t>Broadway</t>
@@ -486,10 +495,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:O115"/>
+  <dimension ref="A1:O117"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="162" zoomScaleNormal="162" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P14" activeCellId="0" sqref="P14"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A102" colorId="64" zoomScale="162" zoomScaleNormal="162" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C105" activeCellId="0" sqref="C105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18"/>
@@ -3339,14 +3348,12 @@
         <v>99</v>
       </c>
       <c r="D103" s="6" t="s">
-        <v>21</v>
+        <v>50</v>
       </c>
       <c r="E103" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="F103" s="6" t="s">
-        <v>24</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="F103" s="5"/>
       <c r="G103" s="5"/>
       <c r="H103" s="5"/>
       <c r="I103" s="5"/>
@@ -3368,17 +3375,13 @@
         <v>100</v>
       </c>
       <c r="D104" s="6" t="s">
-        <v>21</v>
+        <v>50</v>
       </c>
       <c r="E104" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="F104" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="G104" s="6" t="s">
-        <v>24</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="F104" s="5"/>
+      <c r="G104" s="5"/>
       <c r="H104" s="5"/>
       <c r="I104" s="5"/>
       <c r="J104" s="5"/>
@@ -3390,13 +3393,13 @@
     </row>
     <row r="105" customFormat="false" ht="20.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A105" s="2" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="B105" s="3" t="n">
         <v>105</v>
       </c>
       <c r="C105" s="4" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D105" s="6" t="s">
         <v>21</v>
@@ -3419,7 +3422,7 @@
     </row>
     <row r="106" customFormat="false" ht="20.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A106" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B106" s="3" t="n">
         <v>106</v>
@@ -3428,11 +3431,17 @@
         <v>103</v>
       </c>
       <c r="D106" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E106" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="E106" s="5"/>
-      <c r="F106" s="5"/>
-      <c r="G106" s="5"/>
+      <c r="F106" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="G106" s="6" t="s">
+        <v>24</v>
+      </c>
       <c r="H106" s="5"/>
       <c r="I106" s="5"/>
       <c r="J106" s="5"/>
@@ -3444,7 +3453,7 @@
     </row>
     <row r="107" customFormat="false" ht="20.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A107" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B107" s="3" t="n">
         <v>107</v>
@@ -3453,10 +3462,14 @@
         <v>104</v>
       </c>
       <c r="D107" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="E107" s="5"/>
-      <c r="F107" s="5"/>
+        <v>21</v>
+      </c>
+      <c r="E107" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F107" s="6" t="s">
+        <v>24</v>
+      </c>
       <c r="G107" s="5"/>
       <c r="H107" s="5"/>
       <c r="I107" s="5"/>
@@ -3469,13 +3482,13 @@
     </row>
     <row r="108" customFormat="false" ht="20.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A108" s="2" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="B108" s="3" t="n">
         <v>108</v>
       </c>
       <c r="C108" s="4" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D108" s="6" t="s">
         <v>22</v>
@@ -3494,20 +3507,18 @@
     </row>
     <row r="109" customFormat="false" ht="20.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A109" s="2" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="B109" s="3" t="n">
         <v>109</v>
       </c>
       <c r="C109" s="4" t="s">
-        <v>3</v>
+        <v>107</v>
       </c>
       <c r="D109" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="E109" s="6" t="s">
-        <v>24</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="E109" s="5"/>
       <c r="F109" s="5"/>
       <c r="G109" s="5"/>
       <c r="H109" s="5"/>
@@ -3521,20 +3532,18 @@
     </row>
     <row r="110" customFormat="false" ht="20.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A110" s="2" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="B110" s="3" t="n">
         <v>110</v>
       </c>
       <c r="C110" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="D110" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="E110" s="6" t="s">
-        <v>24</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="E110" s="5"/>
       <c r="F110" s="5"/>
       <c r="G110" s="5"/>
       <c r="H110" s="5"/>
@@ -3548,13 +3557,13 @@
     </row>
     <row r="111" customFormat="false" ht="20.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A111" s="2" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="B111" s="3" t="n">
         <v>111</v>
       </c>
       <c r="C111" s="4" t="s">
-        <v>107</v>
+        <v>3</v>
       </c>
       <c r="D111" s="6" t="s">
         <v>2</v>
@@ -3575,13 +3584,13 @@
     </row>
     <row r="112" customFormat="false" ht="20.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A112" s="2" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="B112" s="3" t="n">
         <v>112</v>
       </c>
       <c r="C112" s="4" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D112" s="6" t="s">
         <v>2</v>
@@ -3602,13 +3611,13 @@
     </row>
     <row r="113" customFormat="false" ht="20.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A113" s="2" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="B113" s="3" t="n">
         <v>113</v>
       </c>
       <c r="C113" s="4" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D113" s="6" t="s">
         <v>2</v>
@@ -3629,13 +3638,13 @@
     </row>
     <row r="114" customFormat="false" ht="20.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A114" s="2" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="B114" s="3" t="n">
         <v>114</v>
       </c>
       <c r="C114" s="4" t="s">
-        <v>14</v>
+        <v>111</v>
       </c>
       <c r="D114" s="6" t="s">
         <v>2</v>
@@ -3656,13 +3665,13 @@
     </row>
     <row r="115" customFormat="false" ht="20.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A115" s="2" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="B115" s="3" t="n">
         <v>115</v>
       </c>
       <c r="C115" s="4" t="s">
-        <v>15</v>
+        <v>112</v>
       </c>
       <c r="D115" s="6" t="s">
         <v>2</v>
@@ -3681,6 +3690,60 @@
       <c r="N115" s="5"/>
       <c r="O115" s="5"/>
     </row>
+    <row r="116" customFormat="false" ht="20.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A116" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B116" s="3" t="n">
+        <v>116</v>
+      </c>
+      <c r="C116" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D116" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E116" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F116" s="5"/>
+      <c r="G116" s="5"/>
+      <c r="H116" s="5"/>
+      <c r="I116" s="5"/>
+      <c r="J116" s="5"/>
+      <c r="K116" s="5"/>
+      <c r="L116" s="5"/>
+      <c r="M116" s="5"/>
+      <c r="N116" s="5"/>
+      <c r="O116" s="5"/>
+    </row>
+    <row r="117" customFormat="false" ht="20.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A117" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B117" s="3" t="n">
+        <v>117</v>
+      </c>
+      <c r="C117" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D117" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E117" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F117" s="5"/>
+      <c r="G117" s="5"/>
+      <c r="H117" s="5"/>
+      <c r="I117" s="5"/>
+      <c r="J117" s="5"/>
+      <c r="K117" s="5"/>
+      <c r="L117" s="5"/>
+      <c r="M117" s="5"/>
+      <c r="N117" s="5"/>
+      <c r="O117" s="5"/>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.511805555555555" footer="0.25"/>

</xml_diff>